<commit_message>
update script data point format
Change the scripts to use the format of defining and calling Python functions.
</commit_message>
<xml_diff>
--- a/Non-Augmented_Data/Prompt-Script/Flow_Dataset.xlsx
+++ b/Non-Augmented_Data/Prompt-Script/Flow_Dataset.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wubingyao/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0BA771D7-AAAE-A146-ACDE-10F8C2F28BB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF2E12E8-BFD8-1A4F-AE82-CB2B70517C7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1380" yWindow="500" windowWidth="24900" windowHeight="28300" xr2:uid="{91FCDD96-6842-FF4A-AC96-D02C77CE91C0}"/>
+    <workbookView xWindow="-12720" yWindow="-28120" windowWidth="25360" windowHeight="27980" xr2:uid="{91FCDD96-6842-FF4A-AC96-D02C77CE91C0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,440 +37,31 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="278">
   <si>
-    <t>from openroad import Tech, Design
-from pathlib import path
-tech = Tech()
-# Make sure you have files read into OpenROAD DB
-design = Design(tech)
-floorplan = design.getFloorplan() 
-# Set the floorplan utilization to 50% 
-floorplan_utilization = 50 
-# Set the aspect ratio of the design (height/width) as 0.66 
-floorplan_aspect_ratio = 0.66 
-# Set the spacing between core and die as 10 um
-floorplan_core_spacing = [design.micronToDBU(10) for i in range(4)] 
-# Find the site in lef
-site = floorplan.findSite("site_name")
-floorplan.initFloorplan(floorplan_utilization, floorplan_aspect_ratio,  
-                        floorplan_core_spacing[0], floorplan_core_spacing[1], 
-                        floorplan_core_spacing[2], floorplan_core_spacing[3], site) 
-floorplan.makeTracks()</t>
-  </si>
-  <si>
-    <t>Show me the piece of code to perform floorplanning using a utilization rate of 50% and an aspect ratio of 0.66, and set the spacing between the core and the die to 10 microns</t>
-  </si>
-  <si>
-    <t>from openroad import Tech, Design
-from pathlib import path
-tech = Tech()
-# Make sure you have files read into OpenROAD DB
-design = Design(tech)
-# Place Pins
-params = design.getIOPlacer().getParameters()
-params.setRandSeed(118)
-params.setMinDistanceInTracks(False)
-params.setMinDistance(design.micronToDBU(0))
-params.setCornerAvoidance(design.micronToDBU(0))
-# Place the pins on M6 and M7
-design.getIOPlacer().addHorLayer(design.getTech().getDB().getTech().findLayer("M6"))
-design.getIOPlacer().addVerLayer(design.getTech().getDB().getTech().findLayer("M7"))
-IOPlacer_random_mode = True
-design.getIOPlacer().run(IOPlacer_random_mode)</t>
-  </si>
-  <si>
     <t>How can I place I/O pins of the design block on M6 and M7 layers?</t>
-  </si>
-  <si>
-    <t>from openroad import Tech, Design
-from pathlib import path
-tech = Tech()
-# Make sure you have files read into OpenROAD DB
-design = Design(tech)
-design.readDb("xxx.odb")
-# Global Placement
-gpl = design.getReplace()
-gpl.setTimingDrivenMode(False)
-gpl.setRoutabilityDrivenMode(True)
-gpl.setUniformTargetDensityMode(True)
-# Set the max iteration of global placement to 30 times
-gpl.setInitialPlaceMaxIter(30)
-gpl.setInitDensityPenalityFactor(0.05)
-gpl.doInitialPlace()
-gpl.doNesterovPlace()
-gpl.reset()</t>
   </si>
   <si>
     <t>How can I perform global placement?</t>
   </si>
   <si>
-    <t>from openroad import Tech, Design
-from pathlib import path
-tech = Tech()
-# Make sure you have files read into OpenROAD DB
-design = Design(tech)
-design.readDb("xxx.odb")
-# Global Placement
-gpl = design.getReplace()
-gpl.setTimingDrivenMode(False)
-gpl.setRoutabilityDrivenMode(True)
-gpl.setUniformTargetDensityMode(True)
-# Set the max iteration of global placement to 30 times
-gpl.setInitialPlaceMaxIter(30)
-gpl.setInitDensityPenalityFactor(0.05)
-gpl.doInitialPlace()
-gpl.doNesterovPlace()
-gpl.reset()
-# Macro Placement
-# In OpenROAD, global placement should be performed before macro placement
-macros = [inst for inst in ord.get_db_block().getInsts() if inst.getMaster().isBlock()] 
-if len(macros) &gt; 0:
-  mpl = design.getMacroPlacer()
-  # Set the halo around macros to 5 microns
-  mpl_halo_x, mpl_halo_y = 5, 5
-  mpl.setHalo(mpl_halo_x, mpl_halo_y)
-  # Set the channel width between macros to 5 microns
-  mpl_channel_x, mpl_channel_y = 5, 5
-  mpl.setChannel(mpl_channel_x, mpl_channel_y)
-  # Place the macros using the entire core area
-  core = design.getBlock().getCoreArea()
-  units = design.getBlock().getDbUnitsPerMicron()
-  core_lx = core.xMin() / units
-  core_ly = core.yMin() / units
-  core_ux = core.xMax() / units
-  core_uy = core.yMax() / units
-  design.getMacroPlacer().setFenceRegion(core_lx, core_ly, core_ux, core_uy)
-  # Snap the macro to layer M4 (usually M4)
-  layer = design.getTech().getDB().getTech().findLayer("M4")
-  mpl.setSnapLayer(layer)
-  mpl.placeMacrosCornerMaxWl()</t>
-  </si>
-  <si>
     <t>Place the macros onto the design block</t>
-  </si>
-  <si>
-    <t>from openroad import Tech, Design
-from pathlib import path
-tech = Tech()
-# Make sure you have files read into OpenROAD DB
-design = Design(tech)
-design.readDb("xxx.odb")
-# Detailed Placement
-site = design.getBlock().getRows()[0].getSite()
-max_disp_x = int(design.micronToDBU(0.5) / site.getWidth())
-max_disp_y = int(design.micronToDBU(1) / site.getHeight())
-design.getOpendp().detailedPlacement(max_disp_x, max_disp_y, "", False)</t>
   </si>
   <si>
     <t>Perform detailed placement in OpenROAD</t>
   </si>
   <si>
-    <t>from openroad import Tech, Design
-from pathlib import path
-import openroad as ord
-tech = Tech()
-# Make sure you have files read into OpenROAD DB
-design = Design(tech)
-design.readDb("xxx.odb")
-# Add Filler Cells
-db = ord.get_db()
-filler_masters = list()
-# Filler cell prefix may be different when using different library
-filler_cells_prefix = "filler_.*"
-for lib in db.getLibs():
-  for master in lib.getMasters():
-    master_name = master.getConstName()
-    if re.fullmatch(filler_cells_prefix, master_name) != None:
-      filler_masters.append(master)
-if len(filler_masters) == 0:
-  print("wrong filler cell prefix")
-else:
-  design.getOpendp().fillerPlacement(filler_masters, filler_cells_prefix)</t>
-  </si>
-  <si>
     <t>Add filler cells on the design block</t>
-  </si>
-  <si>
-    <t>from openroad import Tech, Design
-from pathlib import path
-import openroad as ord
-tech = Tech()
-# Make sure you have files read into OpenROAD DB
-design = Design(tech)
-design.readDb("xxx.odb")
-# Power Planning
-# Global Connect
-for net in design.getBlock().getNets():
-  if net.getSigType() == "POWER" or net.getSigType() == "GROUND":
-    net.setSpecial()
-VDD_net = design.getBlock().findNet("VDD")
-VSS_net = design.getBlock().findNet("VSS")
-switched_power = None
-secondary = list()
-if VDD_net == None:
-  VDD_net = odb.dbNet_create(design.getBlock(), "VDD")
-  VDD_net.setSpecial()
-  VDD_net.setSigType("POWER")
-if VSS_net == None:
-  VSS_net = odb.dbNet_create(design.getBlock(), "VSS")
-  VSS_net.setSpecial()
-  VSS_net.setSigType("GROUND")
-design.getBlock().addGlobalConnect(region = None, instPattern = ".*", 
-                                  pinPattern = "^VDD$", net = VDD_net, 
-                                  do_connect = True)
-design.getBlock().addGlobalConnect(region = None, instPattern = ".*",
-                                  pinPattern = "^VDDPE$", net = VDD_net,
-                                  do_connect = True)
-design.getBlock().addGlobalConnect(region = None, instPattern = ".*",
-                                  pinPattern = "^VDDCE$", net = VDD_net,
-                                  do_connect = True)
-design.getBlock().addGlobalConnect(region = None, instPattern = ".*",
-                                  pinPattern = "^VSS$", net = VSS_net, 
-                                  do_connect = True)
-design.getBlock().addGlobalConnect(region = None, instPattern = ".*",
-                                  pinPattern = "^VSSE$", net = VSS_net,
-                                  do_connect = True)
-design.getBlock().globalConnect()
-# Voltage Domains
-pdngen = design.getPdnGen()
-pdngen.setCoreDomain(power = VDD_net, switched_power = switched_power, 
-                    ground = VSS_net, secondary = secondary)
-# Set the width of the PDN ring and the spacing between VDD and VSS rings
-core_ring_width = [design.micronToDBU(5), design.micronToDBU(5)]
-core_ring_spacing = [design.micronToDBU(5), design.micronToDBU(5)]
-core_ring_core_offset = [design.micronToDBU(0) for i in range(4)]
-core_ring_pad_offset = [design.micronToDBU(0) for i in range(4)]
-# When the two layers are parallel, specify the distance between via cuts.
-pdn_cut_pitch = [design.micronToDBU(2) for i in range(2)]
-ring_connect_to_pad_layers = list()
-for layer in design.getTech().getDB().getTech().getLayers():
-  if layer.getType() == "ROUTING":
-    ring_connect_to_pad_layers.append(layer)
-# Define power grid for core
-domains = [pdngen.findDomain("Core")]
-halo = [design.micronToDBU(0) for i in range(4)]
-for domain in domains:
-  pdngen.makeCoreGrid(domain = domain, name = "top_pdn", starts_with = pdn.GROUND, 
-                      pin_layers = [], generate_obstructions = [], powercell = None,
-                      powercontrol = None, powercontrolnetwork = "STAR")
-m1 = design.getTech().getDB().getTech().findLayer("M1")
-m7 = design.getTech().getDB().getTech().findLayer("M7")
-m8 = design.getTech().getDB().getTech().findLayer("M8")
-grid = pdngen.findGrid("top_pdn")
-for g in grid:
-  # Make Ring for the core
-  pdngen.makeRing(grid = g, layer0 = m7, width0 = core_ring_width[0], spacing0 = core_ring_spacing[0],
-                  layer1 = m8, width1 = core_ring_width[0], spacing1 = core_ring_spacing[0],
-                  starts_with = pdn.GRID, offset = core_ring_core_offset, pad_offset = core_ring_pad_offset, extend = False,
-                  pad_pin_layers = ring_connect_to_pad_layers, nets = [])
-  # Add power and ground grid on M1 and attach to cell's VDD/VSS pin
-  pdngen.makeFollowpin(grid = g, layer = m1, 
-                      width = design.micronToDBU(0.07), extend = pdn.CORE)
-  # Create the rest of the power distribution network
-  pdngen.makeStrap(grid = g, layer = m7, width = design.micronToDBU(1.4),
-                  spacing = design.micronToDBU(1.4), pitch = design.micronToDBU(10.8), offset = design.micronToDBU(0),
-                  number_of_straps = 0, snap = False, starts_with = pdn.GRID, extend = pdn.RINGS, nets = [])
-  pdngen.makeConnect(grid = g, layer0 = m1, layer1 = m7, 
-                  cut_pitch_x = pdn_cut_pitch[0], cut_pitch_y = pdn_cut_pitch[1], vias = [], techvias = [],
-                  max_rows = 0, max_columns = 0, ongrid = [], split_cuts = dict(), dont_use_vias = )
-  pdngen.makeConnect(grid = g, layer0 = m7, layer1 = m8,
-                  cut_pitch_x = pdn_cut_pitch[0], cut_pitch_y = pdn_cut_pitch[1], vias = [], techvias = [],
-                  max_rows = 0, max_columns = 0, ongrid = [], split_cuts = dict(), dont_use_vias = )
-pdngen.checkSetup()
-pdngen.buildGrids(False)
-pdngen.writeToDb(True, )
-pdngen.resetShapes()</t>
   </si>
   <si>
     <t>Show me how I can construct power distribution network in OpenROAD</t>
   </si>
   <si>
-    <t>from openroad import Tech, Design
-from pathlib import path
-import openroad as ord
-tech = Tech()
-# Make sure you have files read into OpenROAD DB
-design = Design(tech)
-design.readDb("xxx.odb")
-# Power Planning
-# Global Connect
-for net in design.getBlock().getNets():
-  if net.getSigType() == "POWER" or net.getSigType() == "GROUND":
-    net.setSpecial()
-VDD_net = design.getBlock().findNet("VDD")
-VSS_net = design.getBlock().findNet("VSS")
-switched_power = None
-secondary = list()
-if VDD_net == None:
-  VDD_net = odb.dbNet_create(design.getBlock(), "VDD")
-  VDD_net.setSpecial()
-  VDD_net.setSigType("POWER")
-if VSS_net == None:
-  VSS_net = odb.dbNet_create(design.getBlock(), "VSS")
-  VSS_net.setSpecial()
-  VSS_net.setSigType("GROUND")
-design.getBlock().addGlobalConnect(region = None, instPattern = ".*", 
-                                  pinPattern = "^VDD$", net = VDD_net, 
-                                  do_connect = True)
-design.getBlock().addGlobalConnect(region = None, instPattern = ".*",
-                                  pinPattern = "^VDDPE$", net = VDD_net,
-                                  do_connect = True)
-design.getBlock().addGlobalConnect(region = None, instPattern = ".*",
-                                  pinPattern = "^VDDCE$", net = VDD_net,
-                                  do_connect = True)
-design.getBlock().addGlobalConnect(region = None, instPattern = ".*",
-                                  pinPattern = "^VSS$", net = VSS_net, 
-                                  do_connect = True)
-design.getBlock().addGlobalConnect(region = None, instPattern = ".*",
-                                  pinPattern = "^VSSE$", net = VSS_net,
-                                  do_connect = True)
-design.getBlock().globalConnect()
-# Voltage Domains
-pdngen = design.getPdnGen()
-pdngen.setCoreDomain(power = VDD_net, switched_power = switched_power, 
-                    ground = VSS_net, secondary = secondary)
-# Set the width of the PDN ring and the spacing between VDD and VSS rings
-core_ring_width = [design.micronToDBU(5), design.micronToDBU(5)]
-core_ring_spacing = [design.micronToDBU(5), design.micronToDBU(5)]
-core_ring_core_offset = [design.micronToDBU(0) for i in range(4)]
-core_ring_pad_offset = [design.micronToDBU(0) for i in range(4)]
-# When the two layers are parallel, specify the distance between via cuts.
-pdn_cut_pitch = [design.micronToDBU(2) for i in range(2)]
-ring_connect_to_pad_layers = list()
-for layer in design.getTech().getDB().getTech().getLayers():
-  if layer.getType() == "ROUTING":
-    ring_connect_to_pad_layers.append(layer)
-# Define power grid for core
-domains = [pdngen.findDomain("Core")]
-halo = [design.micronToDBU(0) for i in range(4)]
-for domain in domains:
-  pdngen.makeCoreGrid(domain = domain, name = "top_pdn", starts_with = pdn.GROUND, 
-                      pin_layers = [], generate_obstructions = [], powercell = None,
-                      powercontrol = None, powercontrolnetwork = "STAR")
-m1 = design.getTech().getDB().getTech().findLayer("M1")
-m4 = design.getTech().getDB().getTech().findLayer("M4")
-m7 = design.getTech().getDB().getTech().findLayer("M7")
-m8 = design.getTech().getDB().getTech().findLayer("M8")
-grid = pdngen.findGrid("top_pdn")
-for g in grid:
-  # Make Ring for the core
-  pdngen.makeRing(grid = g, layer0 = m7, width0 = core_ring_width[0], spacing0 = core_ring_spacing[0],
-                  layer1 = m8, width1 = core_ring_width[0], spacing1 = core_ring_spacing[0],
-                  starts_with = pdn.GRID, offset = core_ring_core_offset, pad_offset = core_ring_pad_offset, extend = False,
-                  pad_pin_layers = ring_connect_to_pad_layers, nets = [])
-  # Add power and ground grid on M1 and attach to cell's VDD/VSS pin
-  pdngen.makeFollowpin(grid = g, layer = m1, 
-                      width = design.micronToDBU(0.07), extend = pdn.CORE)
-  # Create the rest of the power delivery network
-  pdngen.makeStrap(grid = g, layer = m4, width = design.micronToDBU(1.2), 
-                  spacing = design.micronToDBU(1.2), pitch = design.micronToDBU(6), offset = design.micronToDBU(0), 
-                  number_of_straps = 0, snap = False, starts_with = pdn.GRID, extend = pdn.CORE, nets = [])
-  pdngen.makeStrap(grid = g, layer = m7, width = design.micronToDBU(1.4),
-                  spacing = design.micronToDBU(1.4), pitch = design.micronToDBU(10.8), offset = design.micronToDBU(0),
-                  number_of_straps = 0, snap = False, starts_with = pdn.GRID, extend = pdn.RINGS, nets = [])
-  pdngen.makeConnect(grid = g, layer0 = m1, layer1 = m4, 
-                  cut_pitch_x = pdn_cut_pitch[0], cut_pitch_y = pdn_cut_pitch[1], vias = [], techvias = [],
-                  max_rows = 0, max_columns = 0, ongrid = [], split_cuts = dict(), dont_use_vias = )
-  pdngen.makeConnect(grid = g, layer0 = m4, layer1 = m7,
-                  cut_pitch_x = pdn_cut_pitch[0], cut_pitch_y = pdn_cut_pitch[1], vias = [], techvias = [],
-                  max_rows = 0, max_columns = 0, ongrid = [], split_cuts = dict(), dont_use_vias = )
-  pdngen.makeConnect(grid = g, layer0 = m7, layer1 = m8,
-                  cut_pitch_x = pdn_cut_pitch[0], cut_pitch_y = pdn_cut_pitch[1], vias = [], techvias = [],
-                  max_rows = 0, max_columns = 0, ongrid = [], split_cuts = dict(), dont_use_vias = )
-# Create power delivery network for macros
-# Set the width of the PDN ring for macros and the spacing between VDD and VSS rings for macros
-macro_ring_width = [design.micronToDBU(2), design.micronToDBU(2)]
-macro_ring_spacing = [design.micronToDBU(2), design.micronToDBU(2)]
-macro_ring_core_offset = [design.micronToDBU(0) for i in range(4)]
-macro_ring_pad_offset = [design.micronToDBU(0) for i in range(4)]
-m5 = design.getTech().getDB().getTech().findLayer("M5")
-m6 = design.getTech().getDB().getTech().findLayer("M6"
-for i in range(len(macros)):
-  for domain in domains:
-    pdngen.makeInstanceGrid(domain = domain, name = "Macro_core_grid_" + str(i),
-                            starts_with = pdn.GROUND, inst = macros[i], halo = halo,
-                            pg_pins_to_boundary = True, default_grid = False, 
-                            generate_obstructions = [], is_bump = False)
-  grid = pdngen.findGrid("Macro_core_grid_" + str(i))
-  for g in grid:
-    pdngen.makeRing(grid = g, layer0 = m5, width0 = macro_ring_width[0], spacing0 = macro_ring_spacing[0],
-                    layer1 = m6, width1 = macro_ring_width[0], spacing1 = macro_ring_spacing[0],
-                    starts_with = pdn.GRID, offset = macro_ring_core_offset, pad_offset = ring_pad_offset, extend = False,
-                    pad_pin_layers = macro_ring_connect_to_pad_layers, nets = [])
-    pdngen.makeStrap(grid = g, layer = m5, width = design.micronToDBU(1.2), 
-                    spacing = design.micronToDBU(1.2), pitch = design.micronToDBU(6), offset = design.micronToDBU(0),
-                    number_of_straps = 0, snap = True, starts_with = pdn.GRID, extend = pdn.RINGS, nets = [])
-    pdngen.makeStrap(grid = g, layer = m6, width = design.micronToDBU(1.2),
-                    spacing = design.micronToDBU(1.2), pitch = design.micronToDBU(6), offset = design.micronToDBU(0),
-                    number_of_straps = 0, snap = True, starts_with = pdn.GRID, extend = pdn.RINGS, nets = [])
-    pdngen.makeConnect(grid = g, layer0 = m4, layer1 = m5,
-                    cut_pitch_x = pdn_cut_pitch[0], cut_pitch_y = pdn_cut_pitch[1], vias = [], techvias = [],
-                    max_rows = 0, max_columns = 0, ongrid = [], split_cuts = dict(), dont_use_vias = )
-    pdngen.makeConnect(grid = g, layer0 = m5, layer1 = m6,
-                    cut_pitch_x = pdn_cut_pitch[0], cut_pitch_y = pdn_cut_pitch[1], vias = [], techvias = [],
-                    max_rows = 0, max_columns = 0, ongrid = [], split_cuts = dict(), dont_use_vias = )
-    pdngen.makeConnect(grid = g, layer0 = m6, layer1 = m7,
-                    cut_pitch_x = pdn_cut_pitch[0], cut_pitch_y = pdn_cut_pitch[1], vias = [], techvias = [],
-                    max_rows = 0, max_columns = 0, ongrid = [], split_cuts = dict(), dont_use_vias = )
-pdngen.checkSetup()
-pdngen.buildGrids(False)
-pdngen.writeToDb(True, )
-pdngen.resetShapes()</t>
-  </si>
-  <si>
     <t>Show me how I can build power distribution network if my design has macros</t>
-  </si>
-  <si>
-    <t>from openroad import Tech, Design
-from pathlib import path
-import openroad as ord
-tech = Tech()
-# Make sure you have files read into OpenROAD DB
-design = Design(tech)
-design.readDb("xxx.odb")
-# Static IR drop Analysis
-psm_obj = design.getPDNSim()
-psm_obj.setNet(ord.Tech().getDB().getChip().getBlock().findNet("VDD"))
-design.evalTclString(f"psm::set_corner [sta::cmd_corner]")
-psm_obj.analyzePowerGrid('', False, '', '')
-drops = psm_obj.getIRDropForLayer(tech.getDB().getTech().findLayer("M1"))</t>
   </si>
   <si>
     <t>How can I perform IR drop analysis on the M1 layer where the pins are located?</t>
   </si>
   <si>
-    <t>from openroad import Tech, Design
-from pathlib import path
-import openroad as ord
-tech = Tech()
-# Make sure you have files read into OpenROAD DB
-design = Design(tech)
-design.readDb("xxx.odb")
-design.evalTclString("report_power")</t>
-  </si>
-  <si>
     <t>Report the switching power, internal power and leakage power of the design</t>
-  </si>
-  <si>
-    <t>from openroad import Tech, Design
-from pathlib import path
-import openroad as ord
-tech = Tech()
-# Make sure you have files read into OpenROAD DB
-design = Design(tech)
-design.readDb("xxx.odb")
-# Global Routing
-signal_low_layer = design.getTech().getDB().getTech().findLayer("M1").getRoutingLevel()
-signal_high_layer = design.getTech().getDB().getTech().findLayer("M6").getRoutingLevel()
-clk_low_layer = design.getTech().getDB().getTech().findLayer("M1").getRoutingLevel()
-clk_high_layer = design.getTech().getDB().getTech().findLayer("M6").getRoutingLevel()
-grt = design.getGlobalRouter()
-grt.setMinRoutingLayer(signal_low_layer)
-grt.setMaxRoutingLayer(signal_high_layer)
-grt.setMinLayerForClock(clk_low_layer)
-grt.setMaxLayerForClock(clk_high_layer)
-grt.setAdjustment(0.5)
-grt.setVerbose(True)
-grt.globalRoute(True)</t>
   </si>
   <si>
     <t>Perform global routing in OpenROAD</t>
@@ -28682,6 +28273,581 @@
     <t xml:space="preserve">Given a synthesized netlist with a clock port named "clk_i", read the library and set the clock period as 20 ns. Perform floorplan and set the bottom-left location of the bounding box of the die as 0,0 and the top-right corner as 45,45. Set the bottom-left corner of the core's bounding box as 5,5 and the top-right corner as 40,40. After floorplanning, place the macros and the standard cells. Place the macros with a bounding box with the bottom-left corner as 5 um,5 um, and the top-right corner as 20 um,25 um. And place each macro at least 5 um to each other, and set a halo region around each macro as 5 um. Set the iteration of the global router as 10 times. In the detailed placement stage, set the maximum displacement at the x-axis as 0 um, and the y-axis as0. After the placement stage, dump the def file and name it "placement.def". </t>
   </si>
   <si>
+    <t>Show me the way to read the Verilog file into OpenROAD</t>
+  </si>
+  <si>
+    <t>How can I read .lef files into OpenROAD?</t>
+  </si>
+  <si>
+    <t>How can I read .lib files into OpenROAD?</t>
+  </si>
+  <si>
+    <t>Perform detailed routing in OpenROAD</t>
+  </si>
+  <si>
+    <t>Show me how I can perform CTS in OpenROAD</t>
+  </si>
+  <si>
+    <t>Get the number of DRVs, cloud size and set the could size to 500 from the detailed router</t>
+  </si>
+  <si>
+    <t>Adjust the setting of vertical length of the IO pin placer to 100</t>
+  </si>
+  <si>
+    <t># Adjust the setting of vertical length of the IO pin placer to 100
+# Get the IO Placer object of the design
+iop = design.getIOPlacer()
+# Get the parameters of the IO Placer
+parameters = iop.getParameters()
+# Set vertical length to 100
+parameters.setVerticalLength(100)</t>
+  </si>
+  <si>
+    <t>Change the setting of horizontal and vertical length of thr IO pin placer to 100</t>
+  </si>
+  <si>
+    <t># Change the setting of horizontal and vertical length of thr IO pin placer to 100
+# Get the IO Placer object of the design
+iop = design.getIOPlacer()
+# Get the parameters of the IO Placer
+parameters = iop.getParameters()
+# Set vertical and horizontal length to 100
+parameters.setVerticalLength(100)
+parameters.setHorizontalLength(100)</t>
+  </si>
+  <si>
+    <t>Get the minimum distance setting of the IO pin placer and set it to 100 if it is 0</t>
+  </si>
+  <si>
+    <t>Get the defined top layer of the IO pin placer</t>
+  </si>
+  <si>
+    <t>Check if the annealing debug mode is on for the IO pin placer and print the configs of the IO pin placer</t>
+  </si>
+  <si>
+    <t>from openroad import Tech, Design
+tech = Tech()
+# Make sure you have files read into OpenROAD DB
+design = Design(tech)
+# Place Pins
+params = design.getIOPlacer().getParameters()
+params.setRandSeed(118)
+params.setMinDistanceInTracks(False)
+params.setMinDistance(design.micronToDBU(0))
+params.setCornerAvoidance(design.micronToDBU(0))
+# Place the pins on M6 and M7
+design.getIOPlacer().addHorLayer(design.getTech().getDB().getTech().findLayer("M6"))
+design.getIOPlacer().addVerLayer(design.getTech().getDB().getTech().findLayer("M7"))
+IOPlacer_random_mode = True
+design.getIOPlacer().run(IOPlacer_random_mode)</t>
+  </si>
+  <si>
+    <t>from openroad import Tech, Design
+tech = Tech()
+# Make sure you have files read into OpenROAD DB
+design = Design(tech)
+design.readDb("xxx.odb")
+# Global Placement
+gpl = design.getReplace()
+gpl.setTimingDrivenMode(False)
+gpl.setRoutabilityDrivenMode(True)
+gpl.setUniformTargetDensityMode(True)
+# Set the max iteration of global placement to 30 times
+gpl.setInitialPlaceMaxIter(30)
+gpl.setInitDensityPenalityFactor(0.05)
+gpl.doInitialPlace()
+gpl.doNesterovPlace()
+gpl.reset()</t>
+  </si>
+  <si>
+    <t>from openroad import Tech, Design
+import openroad as ord
+tech = Tech()
+# Make sure you have files read into OpenROAD DB
+design = Design(tech)
+design.readDb("xxx.odb")
+# Global Routing
+signal_low_layer = design.getTech().getDB().getTech().findLayer("M1").getRoutingLevel()
+signal_high_layer = design.getTech().getDB().getTech().findLayer("M6").getRoutingLevel()
+clk_low_layer = design.getTech().getDB().getTech().findLayer("M1").getRoutingLevel()
+clk_high_layer = design.getTech().getDB().getTech().findLayer("M6").getRoutingLevel()
+grt = design.getGlobalRouter()
+grt.setMinRoutingLayer(signal_low_layer)
+grt.setMaxRoutingLayer(signal_high_layer)
+grt.setMinLayerForClock(clk_low_layer)
+grt.setMaxLayerForClock(clk_high_layer)
+grt.setAdjustment(0.5)
+grt.setVerbose(True)
+grt.globalRoute(True)</t>
+  </si>
+  <si>
+    <t>from openroad import Tech, Design
+import openroad as ord
+tech = Tech()
+# Make sure you have files read into OpenROAD DB
+design = Design(tech)
+design.readDb("xxx.odb")
+design.evalTclString("report_power")</t>
+  </si>
+  <si>
+    <t>from openroad import Tech, Design
+import openroad as ord
+tech = Tech()
+# Make sure you have files read into OpenROAD DB
+design = Design(tech)
+design.readDb("xxx.odb")
+# Static IR drop Analysis
+psm_obj = design.getPDNSim()
+psm_obj.setNet(ord.Tech().getDB().getChip().getBlock().findNet("VDD"))
+design.evalTclString(f"psm::set_corner [sta::cmd_corner]")
+psm_obj.analyzePowerGrid('', False, '', '')
+drops = psm_obj.getIRDropForLayer(tech.getDB().getTech().findLayer("M1"))</t>
+  </si>
+  <si>
+    <t>from openroad import Tech, Design
+import openroad as ord
+tech = Tech()
+# Make sure you have files read into OpenROAD DB
+design = Design(tech)
+design.readDb("xxx.odb")
+# Power Planning
+# Global Connect
+for net in design.getBlock().getNets():
+  if net.getSigType() == "POWER" or net.getSigType() == "GROUND":
+    net.setSpecial()
+VDD_net = design.getBlock().findNet("VDD")
+VSS_net = design.getBlock().findNet("VSS")
+switched_power = None
+secondary = list()
+if VDD_net == None:
+  VDD_net = odb.dbNet_create(design.getBlock(), "VDD")
+  VDD_net.setSpecial()
+  VDD_net.setSigType("POWER")
+if VSS_net == None:
+  VSS_net = odb.dbNet_create(design.getBlock(), "VSS")
+  VSS_net.setSpecial()
+  VSS_net.setSigType("GROUND")
+design.getBlock().addGlobalConnect(region = None, instPattern = ".*", 
+                                  pinPattern = "^VDD$", net = VDD_net, 
+                                  do_connect = True)
+design.getBlock().addGlobalConnect(region = None, instPattern = ".*",
+                                  pinPattern = "^VDDPE$", net = VDD_net,
+                                  do_connect = True)
+design.getBlock().addGlobalConnect(region = None, instPattern = ".*",
+                                  pinPattern = "^VDDCE$", net = VDD_net,
+                                  do_connect = True)
+design.getBlock().addGlobalConnect(region = None, instPattern = ".*",
+                                  pinPattern = "^VSS$", net = VSS_net, 
+                                  do_connect = True)
+design.getBlock().addGlobalConnect(region = None, instPattern = ".*",
+                                  pinPattern = "^VSSE$", net = VSS_net,
+                                  do_connect = True)
+design.getBlock().globalConnect()
+# Voltage Domains
+pdngen = design.getPdnGen()
+pdngen.setCoreDomain(power = VDD_net, switched_power = switched_power, 
+                    ground = VSS_net, secondary = secondary)
+# Set the width of the PDN ring and the spacing between VDD and VSS rings
+core_ring_width = [design.micronToDBU(5), design.micronToDBU(5)]
+core_ring_spacing = [design.micronToDBU(5), design.micronToDBU(5)]
+core_ring_core_offset = [design.micronToDBU(0) for i in range(4)]
+core_ring_pad_offset = [design.micronToDBU(0) for i in range(4)]
+# When the two layers are parallel, specify the distance between via cuts.
+pdn_cut_pitch = [design.micronToDBU(2) for i in range(2)]
+ring_connect_to_pad_layers = list()
+for layer in design.getTech().getDB().getTech().getLayers():
+  if layer.getType() == "ROUTING":
+    ring_connect_to_pad_layers.append(layer)
+# Define power grid for core
+domains = [pdngen.findDomain("Core")]
+halo = [design.micronToDBU(0) for i in range(4)]
+for domain in domains:
+  pdngen.makeCoreGrid(domain = domain, name = "top_pdn", starts_with = pdn.GROUND, 
+                      pin_layers = [], generate_obstructions = [], powercell = None,
+                      powercontrol = None, powercontrolnetwork = "STAR")
+m1 = design.getTech().getDB().getTech().findLayer("M1")
+m4 = design.getTech().getDB().getTech().findLayer("M4")
+m7 = design.getTech().getDB().getTech().findLayer("M7")
+m8 = design.getTech().getDB().getTech().findLayer("M8")
+grid = pdngen.findGrid("top_pdn")
+for g in grid:
+  # Make Ring for the core
+  pdngen.makeRing(grid = g, layer0 = m7, width0 = core_ring_width[0], spacing0 = core_ring_spacing[0],
+                  layer1 = m8, width1 = core_ring_width[0], spacing1 = core_ring_spacing[0],
+                  starts_with = pdn.GRID, offset = core_ring_core_offset, pad_offset = core_ring_pad_offset, extend = False,
+                  pad_pin_layers = ring_connect_to_pad_layers, nets = [])
+  # Add power and ground grid on M1 and attach to cell's VDD/VSS pin
+  pdngen.makeFollowpin(grid = g, layer = m1, 
+                      width = design.micronToDBU(0.07), extend = pdn.CORE)
+  # Create the rest of the power delivery network
+  pdngen.makeStrap(grid = g, layer = m4, width = design.micronToDBU(1.2), 
+                  spacing = design.micronToDBU(1.2), pitch = design.micronToDBU(6), offset = design.micronToDBU(0), 
+                  number_of_straps = 0, snap = False, starts_with = pdn.GRID, extend = pdn.CORE, nets = [])
+  pdngen.makeStrap(grid = g, layer = m7, width = design.micronToDBU(1.4),
+                  spacing = design.micronToDBU(1.4), pitch = design.micronToDBU(10.8), offset = design.micronToDBU(0),
+                  number_of_straps = 0, snap = False, starts_with = pdn.GRID, extend = pdn.RINGS, nets = [])
+  pdngen.makeConnect(grid = g, layer0 = m1, layer1 = m4, 
+                  cut_pitch_x = pdn_cut_pitch[0], cut_pitch_y = pdn_cut_pitch[1], vias = [], techvias = [],
+                  max_rows = 0, max_columns = 0, ongrid = [], split_cuts = dict(), dont_use_vias = )
+  pdngen.makeConnect(grid = g, layer0 = m4, layer1 = m7,
+                  cut_pitch_x = pdn_cut_pitch[0], cut_pitch_y = pdn_cut_pitch[1], vias = [], techvias = [],
+                  max_rows = 0, max_columns = 0, ongrid = [], split_cuts = dict(), dont_use_vias = )
+  pdngen.makeConnect(grid = g, layer0 = m7, layer1 = m8,
+                  cut_pitch_x = pdn_cut_pitch[0], cut_pitch_y = pdn_cut_pitch[1], vias = [], techvias = [],
+                  max_rows = 0, max_columns = 0, ongrid = [], split_cuts = dict(), dont_use_vias = )
+# Create power delivery network for macros
+# Set the width of the PDN ring for macros and the spacing between VDD and VSS rings for macros
+macro_ring_width = [design.micronToDBU(2), design.micronToDBU(2)]
+macro_ring_spacing = [design.micronToDBU(2), design.micronToDBU(2)]
+macro_ring_core_offset = [design.micronToDBU(0) for i in range(4)]
+macro_ring_pad_offset = [design.micronToDBU(0) for i in range(4)]
+m5 = design.getTech().getDB().getTech().findLayer("M5")
+m6 = design.getTech().getDB().getTech().findLayer("M6"
+for i in range(len(macros)):
+  for domain in domains:
+    pdngen.makeInstanceGrid(domain = domain, name = "Macro_core_grid_" + str(i),
+                            starts_with = pdn.GROUND, inst = macros[i], halo = halo,
+                            pg_pins_to_boundary = True, default_grid = False, 
+                            generate_obstructions = [], is_bump = False)
+  grid = pdngen.findGrid("Macro_core_grid_" + str(i))
+  for g in grid:
+    pdngen.makeRing(grid = g, layer0 = m5, width0 = macro_ring_width[0], spacing0 = macro_ring_spacing[0],
+                    layer1 = m6, width1 = macro_ring_width[0], spacing1 = macro_ring_spacing[0],
+                    starts_with = pdn.GRID, offset = macro_ring_core_offset, pad_offset = ring_pad_offset, extend = False,
+                    pad_pin_layers = macro_ring_connect_to_pad_layers, nets = [])
+    pdngen.makeStrap(grid = g, layer = m5, width = design.micronToDBU(1.2), 
+                    spacing = design.micronToDBU(1.2), pitch = design.micronToDBU(6), offset = design.micronToDBU(0),
+                    number_of_straps = 0, snap = True, starts_with = pdn.GRID, extend = pdn.RINGS, nets = [])
+    pdngen.makeStrap(grid = g, layer = m6, width = design.micronToDBU(1.2),
+                    spacing = design.micronToDBU(1.2), pitch = design.micronToDBU(6), offset = design.micronToDBU(0),
+                    number_of_straps = 0, snap = True, starts_with = pdn.GRID, extend = pdn.RINGS, nets = [])
+    pdngen.makeConnect(grid = g, layer0 = m4, layer1 = m5,
+                    cut_pitch_x = pdn_cut_pitch[0], cut_pitch_y = pdn_cut_pitch[1], vias = [], techvias = [],
+                    max_rows = 0, max_columns = 0, ongrid = [], split_cuts = dict(), dont_use_vias = )
+    pdngen.makeConnect(grid = g, layer0 = m5, layer1 = m6,
+                    cut_pitch_x = pdn_cut_pitch[0], cut_pitch_y = pdn_cut_pitch[1], vias = [], techvias = [],
+                    max_rows = 0, max_columns = 0, ongrid = [], split_cuts = dict(), dont_use_vias = )
+    pdngen.makeConnect(grid = g, layer0 = m6, layer1 = m7,
+                    cut_pitch_x = pdn_cut_pitch[0], cut_pitch_y = pdn_cut_pitch[1], vias = [], techvias = [],
+                    max_rows = 0, max_columns = 0, ongrid = [], split_cuts = dict(), dont_use_vias = )
+pdngen.checkSetup()
+pdngen.buildGrids(False)
+pdngen.writeToDb(True, )
+pdngen.resetShapes()</t>
+  </si>
+  <si>
+    <t>from openroad import Tech, Design
+import openroad as ord
+tech = Tech()
+# Make sure you have files read into OpenROAD DB
+design = Design(tech)
+design.readDb("xxx.odb")
+# Power Planning
+# Global Connect
+for net in design.getBlock().getNets():
+  if net.getSigType() == "POWER" or net.getSigType() == "GROUND":
+    net.setSpecial()
+VDD_net = design.getBlock().findNet("VDD")
+VSS_net = design.getBlock().findNet("VSS")
+switched_power = None
+secondary = list()
+if VDD_net == None:
+  VDD_net = odb.dbNet_create(design.getBlock(), "VDD")
+  VDD_net.setSpecial()
+  VDD_net.setSigType("POWER")
+if VSS_net == None:
+  VSS_net = odb.dbNet_create(design.getBlock(), "VSS")
+  VSS_net.setSpecial()
+  VSS_net.setSigType("GROUND")
+design.getBlock().addGlobalConnect(region = None, instPattern = ".*", 
+                                  pinPattern = "^VDD$", net = VDD_net, 
+                                  do_connect = True)
+design.getBlock().addGlobalConnect(region = None, instPattern = ".*",
+                                  pinPattern = "^VDDPE$", net = VDD_net,
+                                  do_connect = True)
+design.getBlock().addGlobalConnect(region = None, instPattern = ".*",
+                                  pinPattern = "^VDDCE$", net = VDD_net,
+                                  do_connect = True)
+design.getBlock().addGlobalConnect(region = None, instPattern = ".*",
+                                  pinPattern = "^VSS$", net = VSS_net, 
+                                  do_connect = True)
+design.getBlock().addGlobalConnect(region = None, instPattern = ".*",
+                                  pinPattern = "^VSSE$", net = VSS_net,
+                                  do_connect = True)
+design.getBlock().globalConnect()
+# Voltage Domains
+pdngen = design.getPdnGen()
+pdngen.setCoreDomain(power = VDD_net, switched_power = switched_power, 
+                    ground = VSS_net, secondary = secondary)
+# Set the width of the PDN ring and the spacing between VDD and VSS rings
+core_ring_width = [design.micronToDBU(5), design.micronToDBU(5)]
+core_ring_spacing = [design.micronToDBU(5), design.micronToDBU(5)]
+core_ring_core_offset = [design.micronToDBU(0) for i in range(4)]
+core_ring_pad_offset = [design.micronToDBU(0) for i in range(4)]
+# When the two layers are parallel, specify the distance between via cuts.
+pdn_cut_pitch = [design.micronToDBU(2) for i in range(2)]
+ring_connect_to_pad_layers = list()
+for layer in design.getTech().getDB().getTech().getLayers():
+  if layer.getType() == "ROUTING":
+    ring_connect_to_pad_layers.append(layer)
+# Define power grid for core
+domains = [pdngen.findDomain("Core")]
+halo = [design.micronToDBU(0) for i in range(4)]
+for domain in domains:
+  pdngen.makeCoreGrid(domain = domain, name = "top_pdn", starts_with = pdn.GROUND, 
+                      pin_layers = [], generate_obstructions = [], powercell = None,
+                      powercontrol = None, powercontrolnetwork = "STAR")
+m1 = design.getTech().getDB().getTech().findLayer("M1")
+m7 = design.getTech().getDB().getTech().findLayer("M7")
+m8 = design.getTech().getDB().getTech().findLayer("M8")
+grid = pdngen.findGrid("top_pdn")
+for g in grid:
+  # Make Ring for the core
+  pdngen.makeRing(grid = g, layer0 = m7, width0 = core_ring_width[0], spacing0 = core_ring_spacing[0],
+                  layer1 = m8, width1 = core_ring_width[0], spacing1 = core_ring_spacing[0],
+                  starts_with = pdn.GRID, offset = core_ring_core_offset, pad_offset = core_ring_pad_offset, extend = False,
+                  pad_pin_layers = ring_connect_to_pad_layers, nets = [])
+  # Add power and ground grid on M1 and attach to cell's VDD/VSS pin
+  pdngen.makeFollowpin(grid = g, layer = m1, 
+                      width = design.micronToDBU(0.07), extend = pdn.CORE)
+  # Create the rest of the power distribution network
+  pdngen.makeStrap(grid = g, layer = m7, width = design.micronToDBU(1.4),
+                  spacing = design.micronToDBU(1.4), pitch = design.micronToDBU(10.8), offset = design.micronToDBU(0),
+                  number_of_straps = 0, snap = False, starts_with = pdn.GRID, extend = pdn.RINGS, nets = [])
+  pdngen.makeConnect(grid = g, layer0 = m1, layer1 = m7, 
+                  cut_pitch_x = pdn_cut_pitch[0], cut_pitch_y = pdn_cut_pitch[1], vias = [], techvias = [],
+                  max_rows = 0, max_columns = 0, ongrid = [], split_cuts = dict(), dont_use_vias = )
+  pdngen.makeConnect(grid = g, layer0 = m7, layer1 = m8,
+                  cut_pitch_x = pdn_cut_pitch[0], cut_pitch_y = pdn_cut_pitch[1], vias = [], techvias = [],
+                  max_rows = 0, max_columns = 0, ongrid = [], split_cuts = dict(), dont_use_vias = )
+pdngen.checkSetup()
+pdngen.buildGrids(False)
+pdngen.writeToDb(True, )
+pdngen.resetShapes()</t>
+  </si>
+  <si>
+    <t>from openroad import Tech, Design
+import openroad as ord
+tech = Tech()
+# Make sure you have files read into OpenROAD DB
+design = Design(tech)
+design.readDb("xxx.odb")
+# Add Filler Cells
+db = ord.get_db()
+filler_masters = list()
+# Filler cell prefix may be different when using different library
+filler_cells_prefix = "filler_.*"
+for lib in db.getLibs():
+  for master in lib.getMasters():
+    master_name = master.getConstName()
+    if re.fullmatch(filler_cells_prefix, master_name) != None:
+      filler_masters.append(master)
+if len(filler_masters) == 0:
+  print("wrong filler cell prefix")
+else:
+  design.getOpendp().fillerPlacement(filler_masters, filler_cells_prefix)</t>
+  </si>
+  <si>
+    <t>from openroad import Tech, Design
+tech = Tech()
+# Make sure you have files read into OpenROAD DB
+design = Design(tech)
+design.readDb("xxx.odb")
+# Detailed Placement
+site = design.getBlock().getRows()[0].getSite()
+max_disp_x = int(design.micronToDBU(0.5) / site.getWidth())
+max_disp_y = int(design.micronToDBU(1) / site.getHeight())
+design.getOpendp().detailedPlacement(max_disp_x, max_disp_y, "", False)</t>
+  </si>
+  <si>
+    <t>from openroad import Tech, Design
+tech = Tech()
+# Make sure you have files read into OpenROAD DB
+design = Design(tech)
+design.readDb("xxx.odb")
+# Global Placement
+gpl = design.getReplace()
+gpl.setTimingDrivenMode(False)
+gpl.setRoutabilityDrivenMode(True)
+gpl.setUniformTargetDensityMode(True)
+# Set the max iteration of global placement to 30 times
+gpl.setInitialPlaceMaxIter(30)
+gpl.setInitDensityPenalityFactor(0.05)
+gpl.doInitialPlace()
+gpl.doNesterovPlace()
+gpl.reset()
+# Macro Placement
+# In OpenROAD, global placement should be performed before macro placement
+macros = [inst for inst in ord.get_db_block().getInsts() if inst.getMaster().isBlock()] 
+if len(macros) &gt; 0:
+  mpl = design.getMacroPlacer()
+  # Set the halo around macros to 5 microns
+  mpl_halo_x, mpl_halo_y = 5, 5
+  mpl.setHalo(mpl_halo_x, mpl_halo_y)
+  # Set the channel width between macros to 5 microns
+  mpl_channel_x, mpl_channel_y = 5, 5
+  mpl.setChannel(mpl_channel_x, mpl_channel_y)
+  # Place the macros using the entire core area
+  core = design.getBlock().getCoreArea()
+  units = design.getBlock().getDbUnitsPerMicron()
+  core_lx = core.xMin() / units
+  core_ly = core.yMin() / units
+  core_ux = core.xMax() / units
+  core_uy = core.yMax() / units
+  design.getMacroPlacer().setFenceRegion(core_lx, core_ly, core_ux, core_uy)
+  # Snap the macro to layer M4 (usually M4)
+  layer = design.getTech().getDB().getTech().findLayer("M4")
+  mpl.setSnapLayer(layer)
+  mpl.placeMacrosCornerMaxWl()</t>
+  </si>
+  <si>
+    <t xml:space="preserve"># Disconnect the nets of the instance 'input1' from the RC network
+# Get the design block
+block = design.getBlock()
+# Find the instance with name 'input1'
+inst = block.findInst('input1')
+# Get the pins of the instance
+pins = inst.getITerms()
+# Iterate through the pins
+for pin in pins:
+    # Get the net connected to the pin
+    net = pin.getNet()
+    if net:
+        # Set the RC disconnected flag for the net
+        net.setRCDisconnected(True)
+</t>
+  </si>
+  <si>
+    <t>Disconnect the nets of the instance 'input1' from the RC network</t>
+  </si>
+  <si>
+    <t>from openroad import Design, Tech
+tech = Tech()
+# Make sure to read all required files
+design = Design(tech)
+# Get PDNGen module
+pdngen_obj = design.getPdnGen()
+# Find the VDD net
+VSS_net = design.getBlock().findNet("VSS")
+# Rip up the VSS grids
+pdn_obj.ripUp(VSS_net)</t>
+  </si>
+  <si>
+    <t>Rip up the VSS grids</t>
+  </si>
+  <si>
+    <t>Rip up the VDD grids</t>
+  </si>
+  <si>
+    <t>from openroad import Design, Tech
+tech = Tech()
+# Make sure to read all required files
+design = Design(tech)
+# Get PDNGen module
+pdngen_obj = design.getPdnGen()
+# Find the VDD net
+VDD_net = design.getBlock().findNet("VDD")
+# Rip up the VDD grids
+pdn_obj.ripUp(VDD_net)</t>
+  </si>
+  <si>
+    <t>from openroad import Tech, Design
+from pathlib import Path
+tech = Tech()
+# Make sure you have .lef files read into OpenROAD DB
+design = Design(tech)
+designDir = Path("design_path")
+design_file_name = "design_filename"
+design_top_module_name = "design_top_module_name"
+verilogFile = designDir/str(design_file_name + ".v")
+design.readVerilog("verilogFile")
+design.link(design_top_module_name)</t>
+  </si>
+  <si>
+    <t>from openroad import Tech, Design
+from pathlib import Path
+tech = Tech()
+# Set file path
+lefDir = Path("lef_path")
+lefFiles = lefDir.glob('*.lef')
+# Modify the technology file postfix for other naming convention
+techLefFiles = lefDir.glob("*.tech.lef")
+# Read library files
+for techLefFile in techLefFiles:
+  tech.readLef(techLefFile.as_posix())
+for lefFile in lefFiles:
+  tech.readLef(lefFile.as_posix())
+design = Design(tech)</t>
+  </si>
+  <si>
+    <t>from openroad import Tech, Design
+from pathlib import Path
+tech = Tech()
+# Set file path
+libDir = Path("lib_path")
+libFiles = libDir.glob("*.lib")
+# Read library files
+for libFile in libFiles:
+  tech.readLiberty(libFile.as_posix())
+design = Design(tech)</t>
+  </si>
+  <si>
+    <t>from openroad import Tech, Design
+import openroad as ord
+tech = Tech()
+# Make sure you have files read into OpenROAD DB
+design = Design(tech)
+design.readDb("xxx.odb")
+# Detailed Routing
+drter = design.getTritonRoute()
+params = drt.ParamStruct()
+params.outputMazeFile = ""
+params.outputDrcFile = ""
+params.outputCmapFile = ""
+params.outputGuideCoverageFile = ""
+params.dbProcessNode = ""
+params.enableViaGen = True
+params.drouteEndIter = 1
+params.viaInPinBottomLayer = ""
+params.viaInPinTopLayer = ""
+params.orSeed = -1
+params.orK = 0
+params.bottomRoutingLayer = "M1"
+params.topRoutingLayer = "M6"
+params.verbose = 1
+params.cleanPatches = True
+params.doPa = True
+params.singleStepDR = False
+params.minAccessPoints = 1
+params.saveGuideUpdates = False
+drter.setParams(params)
+drter.main()</t>
+  </si>
+  <si>
+    <t>from openroad import Tech, Design
+tech = Tech()
+# Make sure you have files read into OpenROAD DB
+design = Design(tech)
+design.readDb("xxx.odb")
+# Clock Tree Synthesis
+design.evalTclString("set_propagated_clock [core_clock]")
+design.evalTclString("set_wire_rc -clock -resistance 0.0435 -capacitance 0.0817")
+design.evalTclString("set_wire_rc -signal -resistance 0.0435 -capacitance 0.0817")
+cts = design.getTritonCts()
+parms = cts.getParms()
+parms.setWireSegmentUnit(20)
+# Can choose different buffer cells for cts
+cts.setBufferList("BUF_X3")
+cts.setRootBuffer("BUF_X3")
+cts.setSinkBuffer("BUF_X3")
+cts.runTritonCts()
+# Detailed Placement
+site = design.getBlock().getRows()[0].getSite()
+max_disp_x = int(design.micronToDBU(0.5) / site.getWidth())
+max_disp_y = int(design.micronToDBU(1) / site.getHeight())
+design.getOpendp().detailedPlacement(max_disp_x, max_disp_y, "", False)</t>
+  </si>
+  <si>
     <t xml:space="preserve">import openroad as ord
 from openroad import Tech, Design
 import os, odb, drt, pdn, re
@@ -28771,121 +28937,50 @@
 </t>
   </si>
   <si>
-    <t>Show me the way to read the Verilog file into OpenROAD</t>
+    <t>If the clock port is called clk_i, how can I set the design clock period to 50 nanoseconds?</t>
   </si>
   <si>
     <t>from openroad import Tech, Design
-from pathlib import path
 tech = Tech()
 # Make sure you have .lef files read into OpenROAD DB
 design = Design(tech)
-designDir = Path("design_path")
-design_file_name = "design_filename"
-design_top_module_name = "design_top_module_name"
-verilogFile = designDir/str(design_file_name + ".v")
-design.readVerilog("verilogFile")
-design.link(design_top_module_name)</t>
+design.evalTclString("create_clock -period 50 [get_ports clk_i] -name core_clock")
+design.evalTclString("set_propagated_clock [all_clocks]")</t>
   </si>
   <si>
-    <t>How can I read .lef files into OpenROAD?</t>
+    <t>def check_annealing_debug_and_print_config():
+    # Get the IO Placer object of the design
+    io_placer = design.getIOPlacer()
+    # Print the configurations of the IO placer
+    io_placer.printConfig()
+    # Return whether the annealing debug is on
+    return io_placer.isAnnealingDebugOn()
+# Call the function to check the annealing debug mode and print the config
+annealing_debug_on = check_annealing_debug_and_print_config()</t>
   </si>
   <si>
-    <t>from openroad import Tech, Design
-from pathlib import path
-tech = Tech()
-# Set file path
-lefDir = Path("lef_path")
-lefFiles = lefDir.glob('*.lef')
-# Modify the technology file postfix for other naming convention
-techLefFiles = lefDir.glob("*.tech.lef")
-# Read library files
-for techLefFile in techLefFiles:
-  tech.readLef(techLefFile.as_posix())
-for lefFile in lefFiles:
-  tech.readLef(lefFile.as_posix())
-design = Design(tech)</t>
+    <t># Get the defined top layer of the IO pin placer
+# Get the IO Placer object of the design
+iop = design.getIOPlacer()
+# Return the top layer
+topLayer = iop.getTopLayer()</t>
   </si>
   <si>
-    <t>How can I read .lib files into OpenROAD?</t>
-  </si>
-  <si>
-    <t>from openroad import Tech, Design
-from pathlib import path
-tech = Tech()
-# Set file path
-libDir = Path("lib_path")
-libFiles = libDir.glob("*.lib")
-# Read library files
-for libFile in libFiles:
-  tech.readLiberty(libFile.as_posix())
-design = Design(tech)</t>
-  </si>
-  <si>
-    <t>Perform detailed routing in OpenROAD</t>
-  </si>
-  <si>
-    <t>from openroad import Tech, Design
-from pathlib import path
-import openroad as ord
-tech = Tech()
-# Make sure you have files read into OpenROAD DB
-design = Design(tech)
-design.readDb("xxx.odb")
-# Detailed Routing
-drter = design.getTritonRoute()
-params = drt.ParamStruct()
-params.outputMazeFile = ""
-params.outputDrcFile = ""
-params.outputCmapFile = ""
-params.outputGuideCoverageFile = ""
-params.dbProcessNode = ""
-params.enableViaGen = True
-params.drouteEndIter = 1
-params.viaInPinBottomLayer = ""
-params.viaInPinTopLayer = ""
-params.orSeed = -1
-params.orK = 0
-params.bottomRoutingLayer = "M1"
-params.topRoutingLayer = "M6"
-params.verbose = 1
-params.cleanPatches = True
-params.doPa = True
-params.singleStepDR = False
-params.minAccessPoints = 1
-params.saveGuideUpdates = False
-drter.setParams(params)
-drter.main()</t>
-  </si>
-  <si>
-    <t>Show me how I can perform CTS in OpenROAD</t>
-  </si>
-  <si>
-    <t>from openroad import Tech, Design
-from pathlib import path
-tech = Tech()
-# Make sure you have files read into OpenROAD DB
-design = Design(tech)
-design.readDb("xxx.odb")
-# Clock Tree Synthesis
-design.evalTclString("set_propagated_clock [core_clock]")
-design.evalTclString("set_wire_rc -clock -resistance 0.0435 -capacitance 0.0817")
-design.evalTclString("set_wire_rc -signal -resistance 0.0435 -capacitance 0.0817")
-cts = design.getTritonCts()
-parms = cts.getParms()
-parms.setWireSegmentUnit(20)
-# Can choose different buffer cells for cts
-cts.setBufferList("BUF_X3")
-cts.setRootBuffer("BUF_X3")
-cts.setSinkBuffer("BUF_X3")
-cts.runTritonCts()
-# Detailed Placement
-site = design.getBlock().getRows()[0].getSite()
-max_disp_x = int(design.micronToDBU(0.5) / site.getWidth())
-max_disp_y = int(design.micronToDBU(1) / site.getHeight())
-design.getOpendp().detailedPlacement(max_disp_x, max_disp_y, "", False)</t>
-  </si>
-  <si>
-    <t>Get the number of DRVs, cloud size and set the could size to 500 from the detailed router</t>
+    <t>def set_min_distance_if_zero(min_distance_value):
+    # Get the IO Placer object of the design
+    iop = design.getIOPlacer()
+    # Get the parameters of the IO Placer
+    parameters = iop.getParameters()
+    # Get the minimum distance
+    min_dist = parameters.getMinDistance()
+    # Set the minimum distance to 100 if it is 0
+    if min_dist == 0:
+        parameters.setMinDistance(min_distance_value)
+    # Set min distance in tracks
+    parameters.setMinDistanceInTracks(True)
+    return min_dist
+# Call the function with the hard-coded min distance value 100
+min_distance = set_min_distance_if_zero(100)</t>
   </si>
   <si>
     <t># Get the number of DRVs, cloud size and set the could size to 500 from the detailed router
@@ -28894,116 +28989,19 @@
 # Get the number of DRVs
 num_drvs = triton_route.getNumDRVs()
 # Set the cloud size to 500
-cloud_size = triton_route.setCloudSize(500)
+cloud_size = triton_route.setCloudSize(500)def get_and_set_drv_and_cloud_size(cloud_size_value):
+    # Get the Triton Route object of the design
+    triton_route = design.getTritonRoute()
+    # Get the number of DRVs
+    num_drvs = triton_route.getNumDRVs()
+    # Set the cloud size to the specified value
+    cloud_size = triton_route.setCloudSize(cloud_size_value)
+    # Return the number of DRVs and cloud size
+    return (num_drvs, cloud_size)
+# Call the function with the hard-coded cloud size value of 500
+drv_and_cloud_size = get_and_set_drv_and_cloud_size(500)
 # Return the number of DRVs and cloud size
 return (num_drvs, cloud_size)</t>
-  </si>
-  <si>
-    <t>Adjust the setting of vertical length of the IO pin placer to 100</t>
-  </si>
-  <si>
-    <t># Adjust the setting of vertical length of the IO pin placer to 100
-# Get the IO Placer object of the design
-iop = design.getIOPlacer()
-# Get the parameters of the IO Placer
-parameters = iop.getParameters()
-# Set vertical length to 100
-parameters.setVerticalLength(100)</t>
-  </si>
-  <si>
-    <t>Change the setting of horizontal and vertical length of thr IO pin placer to 100</t>
-  </si>
-  <si>
-    <t># Change the setting of horizontal and vertical length of thr IO pin placer to 100
-# Get the IO Placer object of the design
-iop = design.getIOPlacer()
-# Get the parameters of the IO Placer
-parameters = iop.getParameters()
-# Set vertical and horizontal length to 100
-parameters.setVerticalLength(100)
-parameters.setHorizontalLength(100)</t>
-  </si>
-  <si>
-    <t>Get the vertical and horizontal length of the setting of the IO pin placer</t>
-  </si>
-  <si>
-    <t># Get the vertical and horizontal length of the setting of the IO pin placer
-# Get the IO Placer object of the design
-iop = design.getIOPlacer()
-# Get the parameters of the IO Placer
-parameters = iop.getParameters()
-# Return the vertical and horizontal length
-return (parameters.getVerticalLength(), parameters.getHorizontalLength())</t>
-  </si>
-  <si>
-    <t>Get the corner avoidance, number of slots and HPWL report of the IO pin placer</t>
-  </si>
-  <si>
-    <t># Get the corner avoidance, number of slots and HPWL report of the IO pin placer
-# Get the IO Placer object of the design
-iop = design.getIOPlacer()
-# Get the parameters of the IO Placer
-parameters = iop.getParameters()
-# Construct the output string with corner avoidance, HPWL report, and number of slots
-output_string = "Corner Avoidance: {}\nHPWL Report: {}\nNumber of slots: {}".format(
-    parameters.getCornerAvoidance(),
-    parameters.getReportHPWL(),
-    parameters.getNumSlots()
-)
-# Return the output string
-return output_string</t>
-  </si>
-  <si>
-    <t>If the clock prot is called clk_i, how can I set the design clock period to 50 nanoseconds?</t>
-  </si>
-  <si>
-    <t>from openroad import Tech, Design
-from pathlib import path
-tech = Tech()
-# Make sure you have .lef files read into OpenROAD DB
-design = Design(tech)
-design.evalTclString("create_clock -period 50 [get_ports clk_i] -name core_clock")
-design.evalTclString("set_propagated_clock [all_clocks]")</t>
-  </si>
-  <si>
-    <t>Get the minimum distance setting of the IO pin placer and set it to 100 if it is 0</t>
-  </si>
-  <si>
-    <t># Get the minimum distance setting of the IO pin placer and set it to 100 if it is 0
-# Get the IO Placer object of the design
-iop = design.getIOPlacer()
-# Get the parameters of the IO Placer
-parameters = iop.getParameters()
-# Set the minimum distance to 100 if it's 0
-min_dist = parameters.getMinDistance()
-if min_dist == 0:
-    parameters.setMinDistance(100)
-# Set min distance in tracks
-parameters.setMinDistanceInTracks(True)
-# Return the minimum distance
-return min_dist</t>
-  </si>
-  <si>
-    <t># Get the defined top layer of the IO pin placer
-# Get the IO Placer object of the design
-iop = design.getIOPlacer()
-# Return the top layer
-return iop.getTopLayer()</t>
-  </si>
-  <si>
-    <t>Get the defined top layer of the IO pin placer</t>
-  </si>
-  <si>
-    <t>Check if the annealing debug mode is on for the IO pin placer and print the configs of the IO pin placer</t>
-  </si>
-  <si>
-    <t># Check if the annealing debug mode is on for the IO pin placer and print the configs of the IO pin placer
-# Get the IO Placer object of the design
-io_placer = design.getIOPlacer()
-# Print the configurations of the IO placer
-io_placer.printConfig()
-# Return whether the annealing debug is on
-return io_placer.isAnnealingDebugOn()</t>
   </si>
 </sst>
 </file>
@@ -29022,6 +29020,7 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -29058,12 +29057,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -29083,9 +29083,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -29123,7 +29123,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -29229,7 +29229,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -29371,7 +29371,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -29381,8 +29381,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50C6DCC4-E178-C34D-A804-6B7E08B60F00}">
   <dimension ref="A1:B139"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A127" workbookViewId="0">
-      <selection activeCell="D149" sqref="D149"/>
+    <sheetView tabSelected="1" topLeftCell="A105" workbookViewId="0">
+      <selection activeCell="A138" sqref="A138:XFD139"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -29392,1114 +29392,1114 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="2" t="s">
-        <v>0</v>
+      <c r="A2" s="3" t="s">
+        <v>34</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>1</v>
+      <c r="B2" s="3" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="2" t="s">
-        <v>2</v>
+      <c r="A3" s="3" t="s">
+        <v>36</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>3</v>
+      <c r="B3" s="3" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="2" t="s">
-        <v>4</v>
+      <c r="A4" s="3" t="s">
+        <v>38</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>5</v>
+      <c r="B4" s="3" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="2" t="s">
-        <v>6</v>
+      <c r="A5" s="3" t="s">
+        <v>40</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>7</v>
+      <c r="B5" s="3" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="2" t="s">
-        <v>8</v>
+      <c r="A6" s="3" t="s">
+        <v>42</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>9</v>
+      <c r="B6" s="3" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="2" t="s">
-        <v>10</v>
+      <c r="A7" s="3" t="s">
+        <v>44</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>11</v>
+      <c r="B7" s="3" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:2">
-      <c r="A8" s="2" t="s">
-        <v>12</v>
+      <c r="A8" s="3" t="s">
+        <v>46</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>13</v>
+      <c r="B8" s="3" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" s="2" t="s">
-        <v>14</v>
+      <c r="A9" s="3" t="s">
+        <v>48</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>15</v>
+      <c r="B9" s="3" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:2">
-      <c r="A10" s="2" t="s">
-        <v>16</v>
+      <c r="A10" s="3" t="s">
+        <v>50</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>17</v>
+      <c r="B10" s="3" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:2">
-      <c r="A11" s="2" t="s">
-        <v>18</v>
+      <c r="A11" s="3" t="s">
+        <v>52</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>19</v>
+      <c r="B11" s="3" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="12" spans="1:2">
-      <c r="A12" s="2" t="s">
-        <v>20</v>
+      <c r="A12" s="3" t="s">
+        <v>54</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>21</v>
+      <c r="B12" s="3" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:2">
-      <c r="A13" s="2" t="s">
-        <v>22</v>
+      <c r="A13" s="3" t="s">
+        <v>56</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>23</v>
+      <c r="B13" s="3" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="3" t="s">
-        <v>26</v>
+        <v>58</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>27</v>
+        <v>59</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="3" t="s">
-        <v>28</v>
+        <v>60</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>29</v>
+        <v>61</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="3" t="s">
-        <v>30</v>
+        <v>62</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>31</v>
+        <v>63</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="3" t="s">
-        <v>32</v>
+        <v>64</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>33</v>
+        <v>65</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="3" t="s">
-        <v>34</v>
+        <v>66</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>35</v>
+        <v>67</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="3" t="s">
-        <v>36</v>
+        <v>68</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>37</v>
+        <v>69</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="3" t="s">
-        <v>38</v>
+        <v>70</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>39</v>
+        <v>71</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="3" t="s">
-        <v>40</v>
+        <v>72</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>41</v>
+        <v>73</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="3" t="s">
-        <v>42</v>
+        <v>74</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>43</v>
+        <v>75</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="3" t="s">
-        <v>44</v>
+        <v>76</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>45</v>
+        <v>77</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="3" t="s">
-        <v>46</v>
+        <v>78</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>47</v>
+        <v>79</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" s="3" t="s">
-        <v>48</v>
+        <v>80</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>49</v>
+        <v>81</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" s="3" t="s">
-        <v>50</v>
+        <v>82</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>51</v>
+        <v>83</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" s="3" t="s">
-        <v>52</v>
+        <v>84</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>53</v>
+        <v>85</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" s="3" t="s">
-        <v>54</v>
+        <v>86</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>55</v>
+        <v>87</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" s="3" t="s">
-        <v>56</v>
+        <v>88</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>57</v>
+        <v>89</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" s="3" t="s">
-        <v>58</v>
+        <v>90</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>59</v>
+        <v>91</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" s="3" t="s">
-        <v>60</v>
+        <v>92</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>61</v>
+        <v>93</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" s="3" t="s">
-        <v>62</v>
+        <v>94</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>63</v>
+        <v>95</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="3" t="s">
-        <v>64</v>
+        <v>96</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>65</v>
+        <v>97</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" s="3" t="s">
-        <v>66</v>
+        <v>98</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>67</v>
+        <v>99</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35" s="3" t="s">
-        <v>68</v>
+        <v>100</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>69</v>
+        <v>101</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" s="3" t="s">
-        <v>70</v>
+        <v>102</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>71</v>
+        <v>103</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" s="3" t="s">
-        <v>72</v>
+        <v>104</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>73</v>
+        <v>105</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" s="3" t="s">
-        <v>74</v>
+        <v>106</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>75</v>
+        <v>107</v>
       </c>
     </row>
     <row r="39" spans="1:2">
       <c r="A39" s="3" t="s">
-        <v>76</v>
+        <v>108</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>77</v>
+        <v>109</v>
       </c>
     </row>
     <row r="40" spans="1:2">
       <c r="A40" s="3" t="s">
-        <v>78</v>
+        <v>110</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>79</v>
+        <v>111</v>
       </c>
     </row>
     <row r="41" spans="1:2">
       <c r="A41" s="3" t="s">
-        <v>80</v>
+        <v>112</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>81</v>
+        <v>113</v>
       </c>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" s="3" t="s">
-        <v>82</v>
+        <v>114</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>83</v>
+        <v>115</v>
       </c>
     </row>
     <row r="43" spans="1:2">
       <c r="A43" s="3" t="s">
-        <v>84</v>
+        <v>116</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>85</v>
+        <v>117</v>
       </c>
     </row>
     <row r="44" spans="1:2">
       <c r="A44" s="3" t="s">
-        <v>86</v>
+        <v>118</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>87</v>
+        <v>119</v>
       </c>
     </row>
     <row r="45" spans="1:2">
       <c r="A45" s="3" t="s">
-        <v>88</v>
+        <v>120</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>89</v>
+        <v>121</v>
       </c>
     </row>
     <row r="46" spans="1:2">
       <c r="A46" s="3" t="s">
-        <v>90</v>
+        <v>122</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>91</v>
+        <v>123</v>
       </c>
     </row>
     <row r="47" spans="1:2">
       <c r="A47" s="3" t="s">
-        <v>92</v>
+        <v>124</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>93</v>
+        <v>125</v>
       </c>
     </row>
     <row r="48" spans="1:2">
       <c r="A48" s="3" t="s">
-        <v>94</v>
+        <v>126</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>95</v>
+        <v>127</v>
       </c>
     </row>
     <row r="49" spans="1:2">
       <c r="A49" s="3" t="s">
-        <v>96</v>
+        <v>128</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>97</v>
+        <v>129</v>
       </c>
     </row>
     <row r="50" spans="1:2">
       <c r="A50" s="3" t="s">
-        <v>98</v>
+        <v>130</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>99</v>
+        <v>131</v>
       </c>
     </row>
     <row r="51" spans="1:2">
       <c r="A51" s="3" t="s">
-        <v>100</v>
+        <v>132</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>101</v>
+        <v>133</v>
       </c>
     </row>
     <row r="52" spans="1:2">
       <c r="A52" s="3" t="s">
-        <v>102</v>
+        <v>134</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>103</v>
+        <v>135</v>
       </c>
     </row>
     <row r="53" spans="1:2">
       <c r="A53" s="3" t="s">
-        <v>104</v>
+        <v>136</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>105</v>
+        <v>137</v>
       </c>
     </row>
     <row r="54" spans="1:2">
       <c r="A54" s="3" t="s">
-        <v>106</v>
+        <v>138</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>107</v>
+        <v>139</v>
       </c>
     </row>
     <row r="55" spans="1:2">
       <c r="A55" s="3" t="s">
-        <v>108</v>
+        <v>140</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>109</v>
+        <v>141</v>
       </c>
     </row>
     <row r="56" spans="1:2">
       <c r="A56" s="3" t="s">
-        <v>110</v>
+        <v>142</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>111</v>
+        <v>143</v>
       </c>
     </row>
     <row r="57" spans="1:2">
       <c r="A57" s="3" t="s">
-        <v>112</v>
+        <v>144</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>113</v>
+        <v>145</v>
       </c>
     </row>
     <row r="58" spans="1:2">
       <c r="A58" s="3" t="s">
-        <v>114</v>
+        <v>146</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>115</v>
+        <v>147</v>
       </c>
     </row>
     <row r="59" spans="1:2">
       <c r="A59" s="3" t="s">
-        <v>116</v>
+        <v>148</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>117</v>
+        <v>149</v>
       </c>
     </row>
     <row r="60" spans="1:2">
       <c r="A60" s="3" t="s">
-        <v>118</v>
+        <v>150</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>119</v>
+        <v>151</v>
       </c>
     </row>
     <row r="61" spans="1:2">
       <c r="A61" s="3" t="s">
-        <v>120</v>
+        <v>152</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>121</v>
+        <v>153</v>
       </c>
     </row>
     <row r="62" spans="1:2">
       <c r="A62" s="3" t="s">
-        <v>122</v>
+        <v>154</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>123</v>
+        <v>155</v>
       </c>
     </row>
     <row r="63" spans="1:2">
       <c r="A63" s="3" t="s">
-        <v>124</v>
+        <v>156</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>125</v>
+        <v>157</v>
       </c>
     </row>
     <row r="64" spans="1:2">
       <c r="A64" s="3" t="s">
-        <v>126</v>
+        <v>158</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>127</v>
+        <v>159</v>
       </c>
     </row>
     <row r="65" spans="1:2">
       <c r="A65" s="3" t="s">
-        <v>128</v>
+        <v>160</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>129</v>
+        <v>161</v>
       </c>
     </row>
     <row r="66" spans="1:2">
       <c r="A66" s="3" t="s">
-        <v>130</v>
+        <v>162</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>131</v>
+        <v>163</v>
       </c>
     </row>
     <row r="67" spans="1:2">
       <c r="A67" s="3" t="s">
-        <v>132</v>
+        <v>164</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>133</v>
+        <v>165</v>
       </c>
     </row>
     <row r="68" spans="1:2">
       <c r="A68" s="3" t="s">
-        <v>134</v>
+        <v>166</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>135</v>
+        <v>167</v>
       </c>
     </row>
     <row r="69" spans="1:2">
       <c r="A69" s="3" t="s">
-        <v>136</v>
+        <v>168</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>137</v>
+        <v>169</v>
       </c>
     </row>
     <row r="70" spans="1:2">
       <c r="A70" s="3" t="s">
-        <v>138</v>
+        <v>170</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>139</v>
+        <v>171</v>
       </c>
     </row>
     <row r="71" spans="1:2">
       <c r="A71" s="3" t="s">
-        <v>140</v>
+        <v>172</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>141</v>
+        <v>173</v>
       </c>
     </row>
     <row r="72" spans="1:2">
       <c r="A72" s="3" t="s">
-        <v>142</v>
+        <v>174</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>143</v>
+        <v>175</v>
       </c>
     </row>
     <row r="73" spans="1:2">
       <c r="A73" s="3" t="s">
-        <v>144</v>
+        <v>176</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>145</v>
+        <v>177</v>
       </c>
     </row>
     <row r="74" spans="1:2">
       <c r="A74" s="3" t="s">
-        <v>146</v>
+        <v>178</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>147</v>
+        <v>179</v>
       </c>
     </row>
     <row r="75" spans="1:2">
       <c r="A75" s="3" t="s">
-        <v>148</v>
+        <v>180</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>149</v>
+        <v>181</v>
       </c>
     </row>
     <row r="76" spans="1:2">
       <c r="A76" s="3" t="s">
-        <v>150</v>
+        <v>182</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>151</v>
+        <v>183</v>
       </c>
     </row>
     <row r="77" spans="1:2">
       <c r="A77" s="3" t="s">
-        <v>152</v>
+        <v>184</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>153</v>
+        <v>185</v>
       </c>
     </row>
     <row r="78" spans="1:2">
       <c r="A78" s="3" t="s">
-        <v>154</v>
+        <v>186</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>155</v>
+        <v>187</v>
       </c>
     </row>
     <row r="79" spans="1:2">
       <c r="A79" s="3" t="s">
-        <v>156</v>
+        <v>188</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>157</v>
+        <v>189</v>
       </c>
     </row>
     <row r="80" spans="1:2">
       <c r="A80" s="3" t="s">
-        <v>158</v>
+        <v>190</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>159</v>
+        <v>191</v>
       </c>
     </row>
     <row r="81" spans="1:2">
       <c r="A81" s="3" t="s">
-        <v>160</v>
+        <v>192</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>161</v>
+        <v>193</v>
       </c>
     </row>
     <row r="82" spans="1:2">
       <c r="A82" s="3" t="s">
-        <v>162</v>
+        <v>194</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>163</v>
+        <v>195</v>
       </c>
     </row>
     <row r="83" spans="1:2">
       <c r="A83" s="3" t="s">
-        <v>164</v>
+        <v>196</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>165</v>
+        <v>197</v>
       </c>
     </row>
     <row r="84" spans="1:2">
       <c r="A84" s="3" t="s">
-        <v>166</v>
+        <v>198</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>167</v>
+        <v>199</v>
       </c>
     </row>
     <row r="85" spans="1:2">
       <c r="A85" s="3" t="s">
-        <v>168</v>
+        <v>200</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>169</v>
+        <v>201</v>
       </c>
     </row>
     <row r="86" spans="1:2">
       <c r="A86" s="3" t="s">
-        <v>170</v>
+        <v>202</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>171</v>
+        <v>203</v>
       </c>
     </row>
     <row r="87" spans="1:2">
       <c r="A87" s="3" t="s">
-        <v>172</v>
+        <v>204</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>173</v>
+        <v>205</v>
       </c>
     </row>
     <row r="88" spans="1:2">
       <c r="A88" s="3" t="s">
-        <v>174</v>
+        <v>206</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>175</v>
+        <v>207</v>
       </c>
     </row>
     <row r="89" spans="1:2">
       <c r="A89" s="3" t="s">
-        <v>176</v>
+        <v>208</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>177</v>
+        <v>209</v>
       </c>
     </row>
     <row r="90" spans="1:2">
       <c r="A90" s="3" t="s">
-        <v>178</v>
+        <v>210</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>179</v>
+        <v>211</v>
       </c>
     </row>
     <row r="91" spans="1:2">
       <c r="A91" s="3" t="s">
-        <v>180</v>
+        <v>212</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>181</v>
+        <v>213</v>
       </c>
     </row>
     <row r="92" spans="1:2">
       <c r="A92" s="3" t="s">
-        <v>182</v>
+        <v>214</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>183</v>
+        <v>215</v>
       </c>
     </row>
     <row r="93" spans="1:2">
       <c r="A93" s="3" t="s">
-        <v>184</v>
+        <v>216</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>185</v>
+        <v>217</v>
       </c>
     </row>
     <row r="94" spans="1:2">
       <c r="A94" s="3" t="s">
-        <v>186</v>
+        <v>218</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>187</v>
+        <v>219</v>
       </c>
     </row>
     <row r="95" spans="1:2">
       <c r="A95" s="3" t="s">
-        <v>188</v>
+        <v>220</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>189</v>
+        <v>221</v>
       </c>
     </row>
     <row r="96" spans="1:2">
       <c r="A96" s="3" t="s">
-        <v>190</v>
+        <v>222</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>191</v>
+        <v>223</v>
       </c>
     </row>
     <row r="97" spans="1:2">
       <c r="A97" s="3" t="s">
-        <v>192</v>
+        <v>224</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>193</v>
+        <v>225</v>
       </c>
     </row>
     <row r="98" spans="1:2">
       <c r="A98" s="3" t="s">
-        <v>194</v>
+        <v>226</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>195</v>
+        <v>227</v>
       </c>
     </row>
     <row r="99" spans="1:2">
       <c r="A99" s="3" t="s">
-        <v>196</v>
+        <v>228</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>197</v>
+        <v>229</v>
       </c>
     </row>
     <row r="100" spans="1:2">
       <c r="A100" s="3" t="s">
-        <v>198</v>
+        <v>230</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>199</v>
+        <v>231</v>
       </c>
     </row>
     <row r="101" spans="1:2">
       <c r="A101" s="3" t="s">
-        <v>200</v>
+        <v>232</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>201</v>
+        <v>233</v>
       </c>
     </row>
     <row r="102" spans="1:2">
       <c r="A102" s="3" t="s">
-        <v>202</v>
+        <v>14</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>203</v>
+        <v>15</v>
       </c>
     </row>
     <row r="103" spans="1:2">
       <c r="A103" s="3" t="s">
-        <v>204</v>
+        <v>16</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>205</v>
+        <v>17</v>
       </c>
     </row>
     <row r="104" spans="1:2">
       <c r="A104" s="3" t="s">
-        <v>206</v>
+        <v>18</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>207</v>
+        <v>19</v>
       </c>
     </row>
     <row r="105" spans="1:2">
       <c r="A105" s="3" t="s">
-        <v>208</v>
+        <v>20</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>209</v>
+        <v>21</v>
       </c>
     </row>
     <row r="106" spans="1:2">
       <c r="A106" s="3" t="s">
-        <v>210</v>
+        <v>22</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>211</v>
+        <v>23</v>
       </c>
     </row>
     <row r="107" spans="1:2">
       <c r="A107" s="3" t="s">
-        <v>212</v>
+        <v>24</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>213</v>
+        <v>25</v>
       </c>
     </row>
     <row r="108" spans="1:2">
       <c r="A108" s="3" t="s">
-        <v>214</v>
+        <v>26</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>215</v>
+        <v>27</v>
       </c>
     </row>
     <row r="109" spans="1:2">
       <c r="A109" s="3" t="s">
-        <v>216</v>
+        <v>28</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>217</v>
+        <v>29</v>
       </c>
     </row>
     <row r="110" spans="1:2">
       <c r="A110" s="3" t="s">
-        <v>218</v>
+        <v>30</v>
       </c>
       <c r="B110" s="3" t="s">
-        <v>219</v>
+        <v>31</v>
       </c>
     </row>
     <row r="111" spans="1:2">
       <c r="A111" s="3" t="s">
-        <v>220</v>
+        <v>32</v>
       </c>
       <c r="B111" s="3" t="s">
-        <v>221</v>
+        <v>33</v>
       </c>
     </row>
     <row r="112" spans="1:2">
-      <c r="A112" s="3" t="s">
-        <v>222</v>
+      <c r="A112" s="4" t="s">
+        <v>260</v>
       </c>
-      <c r="B112" s="3" t="s">
-        <v>223</v>
+      <c r="B112" s="4" t="s">
+        <v>261</v>
       </c>
     </row>
     <row r="113" spans="1:2">
-      <c r="A113" s="3" t="s">
-        <v>224</v>
+      <c r="A113" s="5" t="s">
+        <v>262</v>
       </c>
-      <c r="B113" s="3" t="s">
-        <v>225</v>
+      <c r="B113" s="5" t="s">
+        <v>263</v>
       </c>
     </row>
     <row r="114" spans="1:2">
-      <c r="A114" s="3" t="s">
-        <v>226</v>
+      <c r="A114" s="2" t="s">
+        <v>250</v>
       </c>
-      <c r="B114" s="3" t="s">
-        <v>227</v>
+      <c r="B114" s="2" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="115" spans="1:2">
-      <c r="A115" s="3" t="s">
-        <v>228</v>
+      <c r="A115" s="2" t="s">
+        <v>251</v>
       </c>
-      <c r="B115" s="3" t="s">
-        <v>229</v>
+      <c r="B115" s="2" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="116" spans="1:2">
-      <c r="A116" s="3" t="s">
-        <v>230</v>
+      <c r="A116" s="2" t="s">
+        <v>259</v>
       </c>
-      <c r="B116" s="3" t="s">
-        <v>231</v>
+      <c r="B116" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="117" spans="1:2">
-      <c r="A117" s="3" t="s">
-        <v>232</v>
+      <c r="A117" s="2" t="s">
+        <v>258</v>
       </c>
-      <c r="B117" s="3" t="s">
-        <v>233</v>
+      <c r="B117" s="2" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="118" spans="1:2">
-      <c r="A118" s="3" t="s">
-        <v>234</v>
+      <c r="A118" s="2" t="s">
+        <v>257</v>
       </c>
-      <c r="B118" s="3" t="s">
-        <v>235</v>
+      <c r="B118" s="2" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="119" spans="1:2">
-      <c r="A119" s="3" t="s">
-        <v>236</v>
+      <c r="A119" s="2" t="s">
+        <v>256</v>
       </c>
-      <c r="B119" s="3" t="s">
-        <v>237</v>
+      <c r="B119" s="2" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="120" spans="1:2">
-      <c r="A120" s="3" t="s">
-        <v>238</v>
+      <c r="A120" s="2" t="s">
+        <v>255</v>
       </c>
-      <c r="B120" s="3" t="s">
-        <v>239</v>
+      <c r="B120" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="121" spans="1:2">
-      <c r="A121" s="3" t="s">
-        <v>240</v>
+      <c r="A121" s="2" t="s">
+        <v>254</v>
       </c>
-      <c r="B121" s="3" t="s">
-        <v>241</v>
+      <c r="B121" s="2" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="122" spans="1:2">
-      <c r="A122" s="3" t="s">
-        <v>242</v>
+      <c r="A122" s="2" t="s">
+        <v>253</v>
       </c>
-      <c r="B122" s="3" t="s">
-        <v>243</v>
+      <c r="B122" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="123" spans="1:2">
-      <c r="A123" s="3" t="s">
-        <v>244</v>
+      <c r="A123" s="2" t="s">
+        <v>252</v>
       </c>
-      <c r="B123" s="3" t="s">
-        <v>245</v>
+      <c r="B123" s="2" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="124" spans="1:2">
-      <c r="A124" s="3" t="s">
-        <v>247</v>
+      <c r="A124" s="2" t="s">
+        <v>10</v>
       </c>
-      <c r="B124" s="3" t="s">
-        <v>246</v>
+      <c r="B124" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="125" spans="1:2">
-      <c r="A125" s="3" t="s">
-        <v>249</v>
+      <c r="A125" s="2" t="s">
+        <v>273</v>
       </c>
-      <c r="B125" s="3" t="s">
-        <v>248</v>
+      <c r="B125" s="2" t="s">
+        <v>272</v>
       </c>
     </row>
     <row r="126" spans="1:2">
-      <c r="A126" s="2" t="s">
-        <v>259</v>
+      <c r="A126" s="3" t="s">
+        <v>271</v>
       </c>
-      <c r="B126" s="2" t="s">
-        <v>258</v>
+      <c r="B126" s="3" t="s">
+        <v>236</v>
       </c>
     </row>
     <row r="127" spans="1:2">
       <c r="A127" s="2" t="s">
-        <v>257</v>
+        <v>270</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>256</v>
+        <v>241</v>
       </c>
     </row>
     <row r="128" spans="1:2">
       <c r="A128" s="2" t="s">
-        <v>255</v>
+        <v>269</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>254</v>
+        <v>240</v>
       </c>
     </row>
     <row r="129" spans="1:2">
       <c r="A129" s="2" t="s">
-        <v>253</v>
+        <v>268</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>252</v>
+        <v>239</v>
       </c>
     </row>
     <row r="130" spans="1:2">
       <c r="A130" s="2" t="s">
-        <v>251</v>
+        <v>267</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>250</v>
+        <v>238</v>
       </c>
     </row>
-    <row r="131" spans="1:2" customFormat="1">
-      <c r="A131" s="4" t="s">
-        <v>269</v>
+    <row r="131" spans="1:2">
+      <c r="A131" s="2" t="s">
+        <v>266</v>
       </c>
-      <c r="B131" s="4" t="s">
-        <v>268</v>
+      <c r="B131" s="2" t="s">
+        <v>237</v>
       </c>
     </row>
-    <row r="132" spans="1:2" customFormat="1">
-      <c r="A132" s="4" t="s">
-        <v>267</v>
-      </c>
-      <c r="B132" s="4" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="133" spans="1:2" customFormat="1">
-      <c r="A133" s="4" t="s">
+    <row r="132" spans="1:2">
+      <c r="A132" s="5" t="s">
         <v>265</v>
       </c>
-      <c r="B133" s="4" t="s">
+      <c r="B132" s="5" t="s">
         <v>264</v>
       </c>
     </row>
+    <row r="133" spans="1:2">
+      <c r="A133" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="B133" s="3" t="s">
+        <v>234</v>
+      </c>
+    </row>
     <row r="134" spans="1:2" customFormat="1">
-      <c r="A134" s="4" t="s">
-        <v>263</v>
+      <c r="A134" s="1" t="s">
+        <v>274</v>
       </c>
-      <c r="B134" s="4" t="s">
-        <v>262</v>
+      <c r="B134" s="1" t="s">
+        <v>249</v>
       </c>
     </row>
     <row r="135" spans="1:2" customFormat="1">
-      <c r="A135" s="4" t="s">
-        <v>261</v>
+      <c r="A135" s="1" t="s">
+        <v>275</v>
       </c>
-      <c r="B135" s="4" t="s">
-        <v>260</v>
+      <c r="B135" s="1" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="136" spans="1:2" customFormat="1">
       <c r="A136" s="1" t="s">
-        <v>271</v>
+        <v>276</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>270</v>
+        <v>247</v>
       </c>
     </row>
     <row r="137" spans="1:2" customFormat="1">
-      <c r="A137" s="4" t="s">
-        <v>273</v>
+      <c r="A137" s="1" t="s">
+        <v>277</v>
       </c>
-      <c r="B137" s="4" t="s">
-        <v>272</v>
+      <c r="B137" s="1" t="s">
+        <v>242</v>
       </c>
     </row>
     <row r="138" spans="1:2" customFormat="1">
-      <c r="A138" s="4" t="s">
-        <v>274</v>
+      <c r="A138" s="1" t="s">
+        <v>246</v>
       </c>
-      <c r="B138" s="4" t="s">
-        <v>275</v>
+      <c r="B138" s="1" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="139" spans="1:2" customFormat="1">
-      <c r="A139" s="4" t="s">
-        <v>277</v>
+      <c r="A139" s="1" t="s">
+        <v>244</v>
       </c>
-      <c r="B139" s="4" t="s">
-        <v>276</v>
+      <c r="B139" s="1" t="s">
+        <v>243</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix minor code spacing issue
</commit_message>
<xml_diff>
--- a/Non-Augmented_Data/Prompt-Script/Flow_Dataset.xlsx
+++ b/Non-Augmented_Data/Prompt-Script/Flow_Dataset.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wubingyao/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97125DE0-78AE-3D4E-9424-13B79780BB5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C313397-094C-C145-9BE1-27EEC48F4479}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-12720" yWindow="-28120" windowWidth="25360" windowHeight="27980" xr2:uid="{91FCDD96-6842-FF4A-AC96-D02C77CE91C0}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="28300" xr2:uid="{91FCDD96-6842-FF4A-AC96-D02C77CE91C0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28971,13 +28971,24 @@
 min_distance = set_min_distance_if_zero(100)</t>
   </si>
   <si>
+    <t>from openroad import Design, Tech
+tech = Tech()
+# Make sure to read all required files
+design = Design(tech)
+# Get PDNGen module
+pdngen_obj = design.getPdnGen()
+# Find the VDD net
+VDD_net = design.getBlock().findNet("VDD")
+# Rip up the VDD grids
+pdngen_obj.ripUp(VDD_net)</t>
+  </si>
+  <si>
     <t># Get the number of DRVs, cloud size and set the could size to 500 from the detailed router
 # Get the Triton Route object of the design
 triton_route = design.getTritonRoute()
 # Get the number of DRVs
 num_drvs = triton_route.getNumDRVs()
-# Set the cloud size to 500
-cloud_size = triton_route.setCloudSize(500)def get_and_set_drv_and_cloud_size(cloud_size_value):
+def get_and_set_drv_and_cloud_size(cloud_size_value):
     # Get the Triton Route object of the design
     triton_route = design.getTritonRoute()
     # Get the number of DRVs
@@ -28990,18 +29001,6 @@
 drv_and_cloud_size = get_and_set_drv_and_cloud_size(500)
 # Return the number of DRVs and cloud size
 return (num_drvs, cloud_size)</t>
-  </si>
-  <si>
-    <t>from openroad import Design, Tech
-tech = Tech()
-# Make sure to read all required files
-design = Design(tech)
-# Get PDNGen module
-pdngen_obj = design.getPdnGen()
-# Find the VDD net
-VDD_net = design.getBlock().findNet("VDD")
-# Rip up the VDD grids
-pdngen_obj.ripUp(VDD_net)</t>
   </si>
 </sst>
 </file>
@@ -29059,10 +29058,16 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -29382,11 +29387,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50C6DCC4-E178-C34D-A804-6B7E08B60F00}">
   <dimension ref="A1:B139"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A105" workbookViewId="0">
-      <selection activeCell="C146" sqref="C132:C146"/>
+    <sheetView tabSelected="1" topLeftCell="A134" workbookViewId="0">
+      <selection activeCell="A137" sqref="A137"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="65.33203125" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="16384" width="65.33203125" style="3"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
@@ -29396,903 +29404,903 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
+    <row r="2" spans="1:2" ht="409.6">
+      <c r="A2" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
+    <row r="3" spans="1:2" ht="409.6">
+      <c r="A3" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
+    <row r="4" spans="1:2" ht="409.6">
+      <c r="A4" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
+    <row r="5" spans="1:2" ht="409.6">
+      <c r="A5" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="3" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="s">
+    <row r="6" spans="1:2" ht="409.6">
+      <c r="A6" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="3" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
-      <c r="A7" t="s">
+    <row r="7" spans="1:2" ht="409.6">
+      <c r="A7" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
-      <c r="A8" t="s">
+    <row r="8" spans="1:2" ht="409.6">
+      <c r="A8" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="3" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
-      <c r="A9" t="s">
+    <row r="9" spans="1:2" ht="409.6">
+      <c r="A9" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="3" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
-      <c r="A10" t="s">
+    <row r="10" spans="1:2" ht="409.6">
+      <c r="A10" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="3" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
-      <c r="A11" t="s">
+    <row r="11" spans="1:2" ht="409.6">
+      <c r="A11" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="3" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
-      <c r="A12" t="s">
+    <row r="12" spans="1:2" ht="409.6">
+      <c r="A12" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="3" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
-      <c r="A13" t="s">
+    <row r="13" spans="1:2" ht="409.6">
+      <c r="A13" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="3" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
-      <c r="A14" t="s">
+    <row r="14" spans="1:2" ht="409.6">
+      <c r="A14" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="3" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
-      <c r="A15" t="s">
+    <row r="15" spans="1:2" ht="409.6">
+      <c r="A15" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
-      <c r="A16" t="s">
+    <row r="16" spans="1:2" ht="409.6">
+      <c r="A16" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="3" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
-      <c r="A17" t="s">
+    <row r="17" spans="1:2" ht="409.6">
+      <c r="A17" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="3" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
-      <c r="A18" t="s">
+    <row r="18" spans="1:2" ht="409.6">
+      <c r="A18" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="3" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
-      <c r="A19" t="s">
+    <row r="19" spans="1:2" ht="409.6">
+      <c r="A19" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="3" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
-      <c r="A20" t="s">
+    <row r="20" spans="1:2" ht="409.6">
+      <c r="A20" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="3" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
-      <c r="A21" t="s">
+    <row r="21" spans="1:2" ht="409.6">
+      <c r="A21" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="3" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
-      <c r="A22" t="s">
+    <row r="22" spans="1:2" ht="409.6">
+      <c r="A22" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="3" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
-      <c r="A23" t="s">
+    <row r="23" spans="1:2" ht="409.6">
+      <c r="A23" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="3" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
-      <c r="A24" t="s">
+    <row r="24" spans="1:2" ht="409.6">
+      <c r="A24" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="3" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
-      <c r="A25" t="s">
+    <row r="25" spans="1:2" ht="409.6">
+      <c r="A25" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="3" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
-      <c r="A26" t="s">
+    <row r="26" spans="1:2" ht="409.6">
+      <c r="A26" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="3" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
-      <c r="A27" t="s">
+    <row r="27" spans="1:2" ht="409.6">
+      <c r="A27" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="3" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
-      <c r="A28" t="s">
+    <row r="28" spans="1:2" ht="409.6">
+      <c r="A28" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="3" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
-      <c r="A29" t="s">
+    <row r="29" spans="1:2" ht="409.6">
+      <c r="A29" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="3" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
-      <c r="A30" t="s">
+    <row r="30" spans="1:2" ht="409.6">
+      <c r="A30" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="3" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="31" spans="1:2">
-      <c r="A31" t="s">
+    <row r="31" spans="1:2" ht="409.6">
+      <c r="A31" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="3" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="32" spans="1:2">
-      <c r="A32" t="s">
+    <row r="32" spans="1:2" ht="409.6">
+      <c r="A32" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="3" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
-      <c r="A33" t="s">
+    <row r="33" spans="1:2" ht="409.6">
+      <c r="A33" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="3" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="34" spans="1:2">
-      <c r="A34" t="s">
+    <row r="34" spans="1:2" ht="409.6">
+      <c r="A34" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" s="3" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="35" spans="1:2">
-      <c r="A35" t="s">
+    <row r="35" spans="1:2" ht="409.6">
+      <c r="A35" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" s="3" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="36" spans="1:2">
-      <c r="A36" t="s">
+    <row r="36" spans="1:2" ht="409.6">
+      <c r="A36" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36" s="3" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="37" spans="1:2">
-      <c r="A37" t="s">
+    <row r="37" spans="1:2" ht="409.6">
+      <c r="A37" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B37" s="3" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="38" spans="1:2">
-      <c r="A38" t="s">
+    <row r="38" spans="1:2" ht="409.6">
+      <c r="A38" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B38" s="3" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="39" spans="1:2">
-      <c r="A39" t="s">
+    <row r="39" spans="1:2" ht="409.6">
+      <c r="A39" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B39" s="3" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="40" spans="1:2">
-      <c r="A40" t="s">
+    <row r="40" spans="1:2" ht="409.6">
+      <c r="A40" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B40" s="3" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="41" spans="1:2">
-      <c r="A41" t="s">
+    <row r="41" spans="1:2" ht="409.6">
+      <c r="A41" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B41" s="3" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="42" spans="1:2">
-      <c r="A42" t="s">
+    <row r="42" spans="1:2" ht="409.6">
+      <c r="A42" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B42" s="3" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="43" spans="1:2">
-      <c r="A43" t="s">
+    <row r="43" spans="1:2" ht="409.6">
+      <c r="A43" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B43" s="3" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="44" spans="1:2">
-      <c r="A44" t="s">
+    <row r="44" spans="1:2" ht="409.6">
+      <c r="A44" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B44" s="3" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="45" spans="1:2">
-      <c r="A45" t="s">
+    <row r="45" spans="1:2" ht="409.6">
+      <c r="A45" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B45" s="3" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="46" spans="1:2">
-      <c r="A46" t="s">
+    <row r="46" spans="1:2" ht="409.6">
+      <c r="A46" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B46" s="3" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="47" spans="1:2">
-      <c r="A47" t="s">
+    <row r="47" spans="1:2" ht="409.6">
+      <c r="A47" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B47" s="3" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="48" spans="1:2">
-      <c r="A48" t="s">
+    <row r="48" spans="1:2" ht="409.6">
+      <c r="A48" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B48" s="3" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="49" spans="1:2">
-      <c r="A49" t="s">
+    <row r="49" spans="1:2" ht="409.6">
+      <c r="A49" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B49" s="3" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="50" spans="1:2">
-      <c r="A50" t="s">
+    <row r="50" spans="1:2" ht="409.6">
+      <c r="A50" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B50" s="3" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="51" spans="1:2">
-      <c r="A51" t="s">
+    <row r="51" spans="1:2" ht="409.6">
+      <c r="A51" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B51" s="3" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="52" spans="1:2">
-      <c r="A52" t="s">
+    <row r="52" spans="1:2" ht="409.6">
+      <c r="A52" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B52" s="3" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="53" spans="1:2">
-      <c r="A53" t="s">
+    <row r="53" spans="1:2" ht="409.6">
+      <c r="A53" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B53" s="3" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="54" spans="1:2">
-      <c r="A54" t="s">
+    <row r="54" spans="1:2" ht="409.6">
+      <c r="A54" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B54" s="3" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="55" spans="1:2">
-      <c r="A55" t="s">
+    <row r="55" spans="1:2" ht="409.6">
+      <c r="A55" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B55" s="3" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="56" spans="1:2">
-      <c r="A56" t="s">
+    <row r="56" spans="1:2" ht="409.6">
+      <c r="A56" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B56" s="3" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="57" spans="1:2">
-      <c r="A57" t="s">
+    <row r="57" spans="1:2" ht="409.6">
+      <c r="A57" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B57" s="3" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="58" spans="1:2">
-      <c r="A58" t="s">
+    <row r="58" spans="1:2" ht="409.6">
+      <c r="A58" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B58" s="3" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="59" spans="1:2">
-      <c r="A59" t="s">
+    <row r="59" spans="1:2" ht="409.6">
+      <c r="A59" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B59" s="3" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="60" spans="1:2">
-      <c r="A60" t="s">
+    <row r="60" spans="1:2" ht="409.6">
+      <c r="A60" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B60" s="3" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="61" spans="1:2">
-      <c r="A61" t="s">
+    <row r="61" spans="1:2" ht="409.6">
+      <c r="A61" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B61" s="3" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="62" spans="1:2">
-      <c r="A62" t="s">
+    <row r="62" spans="1:2" ht="409.6">
+      <c r="A62" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B62" s="3" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="63" spans="1:2">
-      <c r="A63" t="s">
+    <row r="63" spans="1:2" ht="409.6">
+      <c r="A63" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B63" s="3" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="64" spans="1:2">
-      <c r="A64" t="s">
+    <row r="64" spans="1:2" ht="409.6">
+      <c r="A64" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B64" s="3" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="65" spans="1:2">
-      <c r="A65" t="s">
+    <row r="65" spans="1:2" ht="409.6">
+      <c r="A65" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="B65" t="s">
+      <c r="B65" s="3" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="66" spans="1:2">
-      <c r="A66" t="s">
+    <row r="66" spans="1:2" ht="409.6">
+      <c r="A66" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B66" s="3" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="67" spans="1:2">
-      <c r="A67" t="s">
+    <row r="67" spans="1:2" ht="409.6">
+      <c r="A67" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="B67" t="s">
+      <c r="B67" s="3" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="68" spans="1:2">
-      <c r="A68" t="s">
+    <row r="68" spans="1:2" ht="409.6">
+      <c r="A68" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="B68" t="s">
+      <c r="B68" s="3" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="69" spans="1:2">
-      <c r="A69" t="s">
+    <row r="69" spans="1:2" ht="409.6">
+      <c r="A69" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="B69" t="s">
+      <c r="B69" s="3" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="70" spans="1:2">
-      <c r="A70" t="s">
+    <row r="70" spans="1:2" ht="409.6">
+      <c r="A70" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="B70" t="s">
+      <c r="B70" s="3" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="71" spans="1:2">
-      <c r="A71" t="s">
+    <row r="71" spans="1:2" ht="409.6">
+      <c r="A71" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="B71" t="s">
+      <c r="B71" s="3" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="72" spans="1:2">
-      <c r="A72" t="s">
+    <row r="72" spans="1:2" ht="409.6">
+      <c r="A72" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="B72" t="s">
+      <c r="B72" s="3" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="73" spans="1:2">
-      <c r="A73" t="s">
+    <row r="73" spans="1:2" ht="409.6">
+      <c r="A73" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="B73" t="s">
+      <c r="B73" s="3" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="74" spans="1:2">
-      <c r="A74" t="s">
+    <row r="74" spans="1:2" ht="409.6">
+      <c r="A74" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="B74" t="s">
+      <c r="B74" s="3" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="75" spans="1:2">
-      <c r="A75" t="s">
+    <row r="75" spans="1:2" ht="409.6">
+      <c r="A75" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="B75" t="s">
+      <c r="B75" s="3" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="76" spans="1:2">
-      <c r="A76" t="s">
+    <row r="76" spans="1:2" ht="409.6">
+      <c r="A76" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="B76" t="s">
+      <c r="B76" s="3" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="77" spans="1:2">
-      <c r="A77" t="s">
+    <row r="77" spans="1:2" ht="409.6">
+      <c r="A77" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="B77" t="s">
+      <c r="B77" s="3" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="78" spans="1:2">
-      <c r="A78" t="s">
+    <row r="78" spans="1:2" ht="409.6">
+      <c r="A78" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="B78" t="s">
+      <c r="B78" s="3" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="79" spans="1:2">
-      <c r="A79" t="s">
+    <row r="79" spans="1:2" ht="409.6">
+      <c r="A79" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="B79" t="s">
+      <c r="B79" s="3" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="80" spans="1:2">
-      <c r="A80" t="s">
+    <row r="80" spans="1:2" ht="409.6">
+      <c r="A80" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="B80" t="s">
+      <c r="B80" s="3" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="81" spans="1:2">
-      <c r="A81" t="s">
+    <row r="81" spans="1:2" ht="409.6">
+      <c r="A81" s="3" t="s">
         <v>192</v>
       </c>
-      <c r="B81" t="s">
+      <c r="B81" s="3" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="82" spans="1:2">
-      <c r="A82" t="s">
+    <row r="82" spans="1:2" ht="409.6">
+      <c r="A82" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="B82" t="s">
+      <c r="B82" s="3" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="83" spans="1:2">
-      <c r="A83" t="s">
+    <row r="83" spans="1:2" ht="409.6">
+      <c r="A83" s="3" t="s">
         <v>196</v>
       </c>
-      <c r="B83" t="s">
+      <c r="B83" s="3" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="84" spans="1:2">
-      <c r="A84" t="s">
+    <row r="84" spans="1:2" ht="409.6">
+      <c r="A84" s="3" t="s">
         <v>198</v>
       </c>
-      <c r="B84" t="s">
+      <c r="B84" s="3" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="85" spans="1:2">
-      <c r="A85" t="s">
+    <row r="85" spans="1:2" ht="409.6">
+      <c r="A85" s="3" t="s">
         <v>200</v>
       </c>
-      <c r="B85" t="s">
+      <c r="B85" s="3" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="86" spans="1:2">
-      <c r="A86" t="s">
+    <row r="86" spans="1:2" ht="409.6">
+      <c r="A86" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="B86" t="s">
+      <c r="B86" s="3" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="87" spans="1:2">
-      <c r="A87" t="s">
+    <row r="87" spans="1:2" ht="409.6">
+      <c r="A87" s="3" t="s">
         <v>204</v>
       </c>
-      <c r="B87" t="s">
+      <c r="B87" s="3" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="88" spans="1:2">
-      <c r="A88" t="s">
+    <row r="88" spans="1:2" ht="409.6">
+      <c r="A88" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="B88" t="s">
+      <c r="B88" s="3" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="89" spans="1:2">
-      <c r="A89" t="s">
+    <row r="89" spans="1:2" ht="409.6">
+      <c r="A89" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="B89" t="s">
+      <c r="B89" s="3" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="90" spans="1:2">
-      <c r="A90" t="s">
+    <row r="90" spans="1:2" ht="409.6">
+      <c r="A90" s="3" t="s">
         <v>210</v>
       </c>
-      <c r="B90" t="s">
+      <c r="B90" s="3" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="91" spans="1:2">
-      <c r="A91" t="s">
+    <row r="91" spans="1:2" ht="409.6">
+      <c r="A91" s="3" t="s">
         <v>212</v>
       </c>
-      <c r="B91" t="s">
+      <c r="B91" s="3" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="92" spans="1:2">
-      <c r="A92" t="s">
+    <row r="92" spans="1:2" ht="409.6">
+      <c r="A92" s="3" t="s">
         <v>214</v>
       </c>
-      <c r="B92" t="s">
+      <c r="B92" s="3" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="93" spans="1:2">
-      <c r="A93" t="s">
+    <row r="93" spans="1:2" ht="409.6">
+      <c r="A93" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="B93" t="s">
+      <c r="B93" s="3" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="94" spans="1:2">
-      <c r="A94" t="s">
+    <row r="94" spans="1:2" ht="409.6">
+      <c r="A94" s="3" t="s">
         <v>218</v>
       </c>
-      <c r="B94" t="s">
+      <c r="B94" s="3" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="95" spans="1:2">
-      <c r="A95" t="s">
+    <row r="95" spans="1:2" ht="409.6">
+      <c r="A95" s="3" t="s">
         <v>220</v>
       </c>
-      <c r="B95" t="s">
+      <c r="B95" s="3" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="96" spans="1:2">
-      <c r="A96" t="s">
+    <row r="96" spans="1:2" ht="409.6">
+      <c r="A96" s="3" t="s">
         <v>222</v>
       </c>
-      <c r="B96" t="s">
+      <c r="B96" s="3" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="97" spans="1:2">
-      <c r="A97" t="s">
+    <row r="97" spans="1:2" ht="409.6">
+      <c r="A97" s="3" t="s">
         <v>224</v>
       </c>
-      <c r="B97" t="s">
+      <c r="B97" s="3" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="98" spans="1:2">
-      <c r="A98" t="s">
+    <row r="98" spans="1:2" ht="409.6">
+      <c r="A98" s="3" t="s">
         <v>226</v>
       </c>
-      <c r="B98" t="s">
+      <c r="B98" s="3" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="99" spans="1:2">
-      <c r="A99" t="s">
+    <row r="99" spans="1:2" ht="409.6">
+      <c r="A99" s="3" t="s">
         <v>228</v>
       </c>
-      <c r="B99" t="s">
+      <c r="B99" s="3" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="100" spans="1:2">
-      <c r="A100" t="s">
+    <row r="100" spans="1:2" ht="409.6">
+      <c r="A100" s="3" t="s">
         <v>230</v>
       </c>
-      <c r="B100" t="s">
+      <c r="B100" s="3" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="101" spans="1:2">
-      <c r="A101" t="s">
+    <row r="101" spans="1:2" ht="409.6">
+      <c r="A101" s="3" t="s">
         <v>232</v>
       </c>
-      <c r="B101" t="s">
+      <c r="B101" s="3" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="102" spans="1:2">
-      <c r="A102" t="s">
+    <row r="102" spans="1:2" ht="409.6">
+      <c r="A102" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B102" t="s">
+      <c r="B102" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="103" spans="1:2">
-      <c r="A103" t="s">
+    <row r="103" spans="1:2" ht="409.6">
+      <c r="A103" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B103" t="s">
+      <c r="B103" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="104" spans="1:2">
-      <c r="A104" t="s">
+    <row r="104" spans="1:2" ht="409.6">
+      <c r="A104" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B104" t="s">
+      <c r="B104" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="105" spans="1:2">
-      <c r="A105" t="s">
+    <row r="105" spans="1:2" ht="409.6">
+      <c r="A105" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B105" t="s">
+      <c r="B105" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="106" spans="1:2">
-      <c r="A106" t="s">
+    <row r="106" spans="1:2" ht="409.6">
+      <c r="A106" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B106" t="s">
+      <c r="B106" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="107" spans="1:2">
-      <c r="A107" t="s">
+    <row r="107" spans="1:2" ht="409.6">
+      <c r="A107" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B107" t="s">
+      <c r="B107" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="108" spans="1:2">
-      <c r="A108" t="s">
+    <row r="108" spans="1:2" ht="409.6">
+      <c r="A108" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B108" t="s">
+      <c r="B108" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="109" spans="1:2">
-      <c r="A109" t="s">
+    <row r="109" spans="1:2" ht="409.6">
+      <c r="A109" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B109" t="s">
+      <c r="B109" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="110" spans="1:2">
-      <c r="A110" t="s">
+    <row r="110" spans="1:2" ht="409.6">
+      <c r="A110" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B110" t="s">
+      <c r="B110" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="111" spans="1:2">
-      <c r="A111" t="s">
+    <row r="111" spans="1:2" ht="409.6">
+      <c r="A111" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B111" t="s">
+      <c r="B111" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="112" spans="1:2">
-      <c r="A112" s="1" t="s">
+    <row r="112" spans="1:2" ht="267">
+      <c r="A112" s="4" t="s">
         <v>260</v>
       </c>
-      <c r="B112" s="1" t="s">
+      <c r="B112" s="4" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="113" spans="1:2">
-      <c r="A113" s="3" t="s">
+    <row r="113" spans="1:2" ht="165">
+      <c r="A113" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="B113" s="3" t="s">
+      <c r="B113" s="1" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="114" spans="1:2">
+    <row r="114" spans="1:2" ht="270">
       <c r="A114" s="2" t="s">
         <v>250</v>
       </c>
@@ -30300,7 +30308,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:2">
+    <row r="115" spans="1:2" ht="270">
       <c r="A115" s="2" t="s">
         <v>251</v>
       </c>
@@ -30308,7 +30316,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:2">
+    <row r="116" spans="1:2" ht="409.6">
       <c r="A116" s="2" t="s">
         <v>259</v>
       </c>
@@ -30316,7 +30324,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="117" spans="1:2">
+    <row r="117" spans="1:2" ht="195">
       <c r="A117" s="2" t="s">
         <v>258</v>
       </c>
@@ -30324,7 +30332,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="118" spans="1:2">
+    <row r="118" spans="1:2" ht="328">
       <c r="A118" s="2" t="s">
         <v>257</v>
       </c>
@@ -30332,7 +30340,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="119" spans="1:2">
+    <row r="119" spans="1:2" ht="409.6">
       <c r="A119" s="2" t="s">
         <v>256</v>
       </c>
@@ -30340,7 +30348,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="120" spans="1:2">
+    <row r="120" spans="1:2" ht="409.6">
       <c r="A120" s="2" t="s">
         <v>255</v>
       </c>
@@ -30348,7 +30356,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="121" spans="1:2">
+    <row r="121" spans="1:2" ht="225">
       <c r="A121" s="2" t="s">
         <v>254</v>
       </c>
@@ -30356,7 +30364,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="122" spans="1:2">
+    <row r="122" spans="1:2" ht="135">
       <c r="A122" s="2" t="s">
         <v>253</v>
       </c>
@@ -30364,7 +30372,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="123" spans="1:2">
+    <row r="123" spans="1:2" ht="314">
       <c r="A123" s="2" t="s">
         <v>252</v>
       </c>
@@ -30372,7 +30380,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="124" spans="1:2">
+    <row r="124" spans="1:2" ht="409.6">
       <c r="A124" s="2" t="s">
         <v>10</v>
       </c>
@@ -30380,7 +30388,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="125" spans="1:2">
+    <row r="125" spans="1:2" ht="105">
       <c r="A125" s="2" t="s">
         <v>272</v>
       </c>
@@ -30388,15 +30396,15 @@
         <v>271</v>
       </c>
     </row>
-    <row r="126" spans="1:2">
-      <c r="A126" t="s">
+    <row r="126" spans="1:2" ht="409.6">
+      <c r="A126" s="3" t="s">
         <v>270</v>
       </c>
-      <c r="B126" t="s">
+      <c r="B126" s="3" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="127" spans="1:2">
+    <row r="127" spans="1:2" ht="370">
       <c r="A127" s="2" t="s">
         <v>269</v>
       </c>
@@ -30404,7 +30412,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="128" spans="1:2">
+    <row r="128" spans="1:2" ht="409.6">
       <c r="A128" s="2" t="s">
         <v>268</v>
       </c>
@@ -30412,7 +30420,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="129" spans="1:2">
+    <row r="129" spans="1:2" ht="165">
       <c r="A129" s="2" t="s">
         <v>267</v>
       </c>
@@ -30420,7 +30428,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="130" spans="1:2">
+    <row r="130" spans="1:2" ht="225">
       <c r="A130" s="2" t="s">
         <v>266</v>
       </c>
@@ -30428,7 +30436,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="131" spans="1:2">
+    <row r="131" spans="1:2" ht="195">
       <c r="A131" s="2" t="s">
         <v>265</v>
       </c>
@@ -30436,67 +30444,67 @@
         <v>237</v>
       </c>
     </row>
-    <row r="132" spans="1:2" ht="384">
-      <c r="A132" s="4" t="s">
-        <v>277</v>
+    <row r="132" spans="1:2" ht="165">
+      <c r="A132" s="1" t="s">
+        <v>276</v>
       </c>
-      <c r="B132" s="3" t="s">
+      <c r="B132" s="1" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="133" spans="1:2">
-      <c r="A133" t="s">
+    <row r="133" spans="1:2" ht="409.6">
+      <c r="A133" s="3" t="s">
         <v>235</v>
       </c>
-      <c r="B133" t="s">
+      <c r="B133" s="3" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="134" spans="1:2">
-      <c r="A134" s="1" t="s">
+    <row r="134" spans="1:2" ht="169">
+      <c r="A134" s="4" t="s">
         <v>273</v>
       </c>
-      <c r="B134" s="1" t="s">
+      <c r="B134" s="4" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="135" spans="1:2">
-      <c r="A135" s="1" t="s">
+    <row r="135" spans="1:2" ht="99">
+      <c r="A135" s="4" t="s">
         <v>274</v>
       </c>
-      <c r="B135" s="1" t="s">
+      <c r="B135" s="4" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="136" spans="1:2">
-      <c r="A136" s="1" t="s">
+    <row r="136" spans="1:2" ht="294">
+      <c r="A136" s="4" t="s">
         <v>275</v>
       </c>
-      <c r="B136" s="1" t="s">
+      <c r="B136" s="4" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="137" spans="1:2">
-      <c r="A137" s="1" t="s">
-        <v>276</v>
+    <row r="137" spans="1:2" ht="359">
+      <c r="A137" s="4" t="s">
+        <v>277</v>
       </c>
-      <c r="B137" s="1" t="s">
+      <c r="B137" s="4" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="138" spans="1:2">
-      <c r="A138" s="1" t="s">
+    <row r="138" spans="1:2" ht="155">
+      <c r="A138" s="4" t="s">
         <v>246</v>
       </c>
-      <c r="B138" s="1" t="s">
+      <c r="B138" s="4" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="139" spans="1:2">
-      <c r="A139" s="1" t="s">
+    <row r="139" spans="1:2" ht="141">
+      <c r="A139" s="4" t="s">
         <v>244</v>
       </c>
-      <c r="B139" s="1" t="s">
+      <c r="B139" s="4" t="s">
         <v>243</v>
       </c>
     </row>

</xml_diff>